<commit_message>
Created file that trains and saves each model
</commit_message>
<xml_diff>
--- a/predict_from_audio/prediction.xlsx
+++ b/predict_from_audio/prediction.xlsx
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -521,16 +521,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -545,16 +545,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.42</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -565,20 +565,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.84</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +593,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.86</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -617,10 +617,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -641,16 +641,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.26</v>
+        <v>0.3386495073309164</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2</v>
+        <v>0.3306152359259172</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.14</v>
+        <v>0.3307352567431665</v>
       </c>
     </row>
     <row r="9">
@@ -665,16 +665,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.5600000000000001</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -685,20 +685,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5600000000000001</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.42</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -713,16 +713,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.06</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.82</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -737,16 +737,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.04</v>
+        <v>0.6653830943429145</v>
       </c>
       <c r="D12" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.86</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02</v>
+        <v>0.3346169056570855</v>
       </c>
     </row>
     <row r="13">
@@ -761,16 +761,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.44</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -809,13 +809,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -833,16 +833,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.58</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>0.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -857,16 +857,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0.14</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.58</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -881,16 +881,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>0.38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -905,16 +905,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.82</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -929,16 +929,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.34</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -949,20 +949,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.28</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -973,20 +973,20 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.3</v>
+        <v>0.6685935153207773</v>
       </c>
       <c r="D22" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.1</v>
+        <v>0.3314064846792227</v>
       </c>
       <c r="F22" t="n">
-        <v>0.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1001,16 +1001,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1025,16 +1025,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.54</v>
+        <v>0.6671008803626376</v>
       </c>
       <c r="D24" t="n">
-        <v>0.14</v>
+        <v>0.3328991196373624</v>
       </c>
       <c r="E24" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1049,16 +1049,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.02</v>
+        <v>0.671362379512858</v>
       </c>
       <c r="D25" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0.86</v>
+        <v>0.3286376204871418</v>
       </c>
       <c r="F25" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1073,16 +1073,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated requirements to test on another machine
</commit_message>
<xml_diff>
--- a/predict_from_audio/prediction.xlsx
+++ b/predict_from_audio/prediction.xlsx
@@ -641,16 +641,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3386495073309164</v>
+        <v>0.3386495067941354</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3306152359259172</v>
+        <v>0.330615235908261</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3307352567431665</v>
+        <v>0.3307352572976036</v>
       </c>
     </row>
     <row r="9">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6653830943429145</v>
+        <v>0.6653830954784715</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -746,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3346169056570855</v>
+        <v>0.3346169045215285</v>
       </c>
     </row>
     <row r="13">
@@ -977,13 +977,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.6685935153207773</v>
+        <v>0.6685935168360657</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.3314064846792227</v>
+        <v>0.3314064831639343</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1025,10 +1025,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.6671008803626376</v>
+        <v>0.6671008805885427</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3328991196373624</v>
+        <v>0.3328991194114574</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1049,13 +1049,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.671362379512858</v>
+        <v>0.6713623762974522</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0.3286376204871418</v>
+        <v>0.3286376237025478</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
changed so different models can be called
</commit_message>
<xml_diff>
--- a/predict_from_audio/prediction.xlsx
+++ b/predict_from_audio/prediction.xlsx
@@ -493,20 +493,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
         <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.6665308908294946</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.3334691091705055</v>
       </c>
     </row>
     <row r="4">
@@ -565,14 +565,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.3151691432172188</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.6848308567827812</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -589,17 +589,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0.3264818596618402</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.3273263381045693</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.3461918022335906</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -613,11 +613,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.3435351089752017</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.6564648910247981</v>
       </c>
     </row>
     <row r="8">
@@ -641,16 +641,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3386495073309164</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3306152359259172</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3307352567431665</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -685,20 +685,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.6669168179794867</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.3330831820205133</v>
       </c>
     </row>
     <row r="11">
@@ -709,14 +709,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
         <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -733,20 +733,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6653830943429145</v>
+        <v>0.3264689577657587</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.3421267112218081</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3346169056570855</v>
+        <v>0.3314043310124331</v>
       </c>
     </row>
     <row r="13">
@@ -764,13 +764,13 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0.6704549760390368</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.3295450239609632</v>
       </c>
     </row>
     <row r="14">
@@ -781,17 +781,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>0.6782308396048843</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>0.3217691603951158</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -805,17 +805,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -829,17 +829,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -853,17 +853,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -877,17 +877,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -901,17 +901,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>0.6745626536237902</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0.3254373463762097</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -929,7 +929,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0.3511738586968672</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>0.6488261413031329</v>
       </c>
     </row>
     <row r="21">
@@ -959,10 +959,10 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>0.334688955108254</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>0.6653110448917461</v>
       </c>
     </row>
     <row r="22">
@@ -977,13 +977,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.6685935153207773</v>
+        <v>0.6698870206226143</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>0.3301129793773858</v>
       </c>
       <c r="E22" t="n">
-        <v>0.3314064846792227</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -997,20 +997,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>0.3578590534864374</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>0.6421409465135626</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1025,10 +1025,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.6671008803626376</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3328991196373624</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1049,13 +1049,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.671362379512858</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>0.3286376204871418</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1073,16 +1073,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>0.3275421410722453</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>0.3365458514056789</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>0.3359120075220757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added audio and changed multiple prediction
</commit_message>
<xml_diff>
--- a/predict_from_audio/prediction.xlsx
+++ b/predict_from_audio/prediction.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,6 @@
           <t>emotion to predict</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>result</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>angry</t>
@@ -493,20 +488,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.9999999999999958</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>4.291846626024645e-15</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>6.66485617840923e-26</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>3.548520108061694e-31</v>
       </c>
     </row>
     <row r="3">
@@ -521,16 +516,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6665308908294946</v>
+        <v>0.9999999999948537</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>5.146324637887233e-12</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>2.810826813893951e-30</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3334691091705055</v>
+        <v>5.268669145896358e-29</v>
       </c>
     </row>
     <row r="4">
@@ -541,20 +536,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.1028777073031261</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.8529391729352254</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>5.034425655902e-10</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.04418311925820596</v>
       </c>
     </row>
     <row r="5">
@@ -565,20 +560,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3151691432172188</v>
+        <v>0.7666623952473265</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6848308567827812</v>
+        <v>0.2333357142873389</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1.753678623225305e-08</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1.872928548387014e-06</v>
       </c>
     </row>
     <row r="6">
@@ -589,20 +584,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3264818596618402</v>
+        <v>0.999999980545106</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3273263381045693</v>
+        <v>1.730659158882568e-08</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3461918022335906</v>
+        <v>4.379235247356553e-16</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>2.148301860307265e-09</v>
       </c>
     </row>
     <row r="7">
@@ -613,20 +608,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.3435351089752017</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1.924163704260329e-17</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>2.294331200125262e-25</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6564648910247981</v>
+        <v>2.205737654997553e-20</v>
       </c>
     </row>
     <row r="8">
@@ -637,20 +632,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>7.160066741041603e-05</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.9938370957247582</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>4.655726129925718e-12</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.006091303603175372</v>
       </c>
     </row>
     <row r="9">
@@ -661,20 +656,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>7.767771464208086e-11</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.9998186783651475</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>3.704340991320492e-10</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.0001813211867407489</v>
       </c>
     </row>
     <row r="10">
@@ -685,20 +680,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6669168179794867</v>
+        <v>0.0002001987242701397</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.9997988591267064</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>3.891104573591962e-10</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3330831820205133</v>
+        <v>9.417599129913047e-07</v>
       </c>
     </row>
     <row r="11">
@@ -713,16 +708,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>7.285877384671724e-05</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.9998972816141034</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>6.163826617593398e-11</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>2.985955041153062e-05</v>
       </c>
     </row>
     <row r="12">
@@ -737,16 +732,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.3264689577657587</v>
+        <v>0.0001941658518078025</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3421267112218081</v>
+        <v>0.885309060400899</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>8.211051501150986e-10</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3314043310124331</v>
+        <v>0.1144967729261881</v>
       </c>
     </row>
     <row r="13">
@@ -761,16 +756,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.001205930314508531</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6704549760390368</v>
+        <v>0.9987940151248954</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>5.321840327646175e-08</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3295450239609632</v>
+        <v>1.342192599378953e-09</v>
       </c>
     </row>
     <row r="14">
@@ -781,20 +776,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.6782308396048843</v>
+        <v>3.655757449281229e-08</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3217691603951158</v>
+        <v>2.577855951990804e-10</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>0.9999124400639006</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>8.752312073935968e-05</v>
       </c>
     </row>
     <row r="15">
@@ -805,20 +800,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>2.972498185852568e-13</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>7.483698164820451e-13</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.9999999926922711</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>7.306683212888786e-09</v>
       </c>
     </row>
     <row r="16">
@@ -829,20 +824,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1.818326810761002e-09</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>1.88864279690199e-07</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>0.9999789101249372</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>2.089919245621273e-05</v>
       </c>
     </row>
     <row r="17">
@@ -853,20 +848,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>0.0006363943832354439</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>5.097935127992823e-07</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.7139565301732967</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.285406565649955</v>
       </c>
     </row>
     <row r="18">
@@ -881,16 +876,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0.0003172675327794079</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>0.0001624648103621018</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.04522183670170381</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>0.9542984309551547</v>
       </c>
     </row>
     <row r="19">
@@ -901,20 +896,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>5.545264395613459e-28</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6745626536237902</v>
+        <v>1.463972414254795e-19</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3254373463762097</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>3.175274972802759e-27</v>
       </c>
     </row>
     <row r="20">
@@ -929,16 +924,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.3511738586968672</v>
+        <v>0.002231696413647554</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>0.9974179285381959</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>5.738162865051805e-08</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6488261413031329</v>
+        <v>0.0003503176665278402</v>
       </c>
     </row>
     <row r="21">
@@ -953,16 +948,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1.385949559080319e-11</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>2.655396857779116e-06</v>
       </c>
       <c r="E21" t="n">
-        <v>0.334688955108254</v>
+        <v>1.321731641938074e-13</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6653110448917461</v>
+        <v>0.9999973445891506</v>
       </c>
     </row>
     <row r="22">
@@ -973,20 +968,20 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.6698870206226143</v>
+        <v>2.754139667201018e-08</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3301129793773858</v>
+        <v>2.950762397383278e-09</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>7.758754129680849e-08</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>0.9999998919202996</v>
       </c>
     </row>
     <row r="23">
@@ -997,20 +992,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.3578590534864374</v>
+        <v>7.933802066873205e-08</v>
       </c>
       <c r="D23" t="n">
-        <v>0.6421409465135626</v>
+        <v>2.964548334569894e-06</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>0.002664593551422074</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>0.9973323625622228</v>
       </c>
     </row>
     <row r="24">
@@ -1021,20 +1016,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0.001097362606637019</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>5.848605007532611e-06</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1.842473284582486e-07</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>0.9988966045410269</v>
       </c>
     </row>
     <row r="25">
@@ -1045,20 +1040,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>0.00227936324341661</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>0.0006771221581906856</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1.563432639650271e-10</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>0.9970435144420494</v>
       </c>
     </row>
     <row r="26">
@@ -1069,20 +1064,788 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.3275421410722453</v>
+        <v>1.059517386278515e-08</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>0.001041190368569997</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3365458514056789</v>
+        <v>3.398141903940196e-05</v>
       </c>
       <c r="F26" t="n">
-        <v>0.3359120075220757</v>
+        <v>0.9989248176172167</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>angry</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.9995721705358902</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0004277053458163146</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.240794930920694e-07</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3.880033353820926e-11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>angry</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.9999990763143342</v>
+      </c>
+      <c r="D28" t="n">
+        <v>9.206551458264538e-07</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2.895861708235209e-09</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1.346580551683429e-10</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0.9987928457965177</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.001131363067335202</v>
+      </c>
+      <c r="E29" t="n">
+        <v>7.52820697739485e-05</v>
+      </c>
+      <c r="F29" t="n">
+        <v>5.090663732402273e-07</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0.007409017009692965</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.03906467134675482</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.02094113254565224</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.9325851790979</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1.886445523589289e-08</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0727366312636923</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.6959178584831803</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.2313454913886721</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0.959734283109663</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.03464889177353165</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.001456493974241639</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.004160331142563724</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>7.661429068461271e-05</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.006508287310060995</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.9923101257946085</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.001104972604645775</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1.271436182264907e-09</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.006220614286581693</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.9902612076977917</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.00351817674419033</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>angry</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.9999981530185628</v>
+      </c>
+      <c r="D35" t="n">
+        <v>5.841941782252971e-07</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.271615089490744e-09</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.261515643896474e-06</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>angry</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0.9539258530745879</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.04607403663865661</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.526945979541792e-11</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1.102614859899988e-07</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1.5981035990305e-08</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.008761163441396354</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.242975578146528e-06</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.9912375776019895</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0.004799249855495546</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.9817976558239718</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6.438453634667692e-05</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.01333870978418593</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0.001534786125160449</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.3044128215254032</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.5033205107084728</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.1907318816409633</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1.313337767115214e-05</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.7244059500682311</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.2507082737100196</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.02487264284407821</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>0.0001853635227671776</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.595294055793272</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.0761799787898487</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.3283406018941121</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0.1403318805639651</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.1233044973016834</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.5957044938677239</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.1406591282666275</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>angry</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.007871794831014104</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.6128756203690255</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.00011859168776166</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.3791339931121985</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>angry</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0.933342097924862</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.06404864795599134</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1.469181154394465e-05</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.002594562307602802</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0.9999339846265671</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3.391343729260749e-05</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3.098749641246511e-05</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1.114439727982079e-06</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0.9815260565074053</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.01842195184277194</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1.301744078155718e-05</v>
+      </c>
+      <c r="F46" t="n">
+        <v>3.897420904106367e-05</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>6.834589457218006e-05</v>
+      </c>
+      <c r="D47" t="n">
+        <v>3.18409901194095e-07</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.000173686538987348</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.9997576491565392</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0.00112738871308322</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.0006072808962604886</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.0001837692321294081</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.998081561158527</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0.0448076378585431</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.01209983737535265</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.0004834905551472906</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.942609034210957</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>0.8336064826098039</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.1505400630220914</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.0001059544595925266</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.01574749990851225</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>angry</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>6.551771406901146e-07</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1.356957952646745e-09</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.9999993434657899</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1.113762560245061e-13</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>angry</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>0.2332444467004595</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.0003675825981806465</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.7663867704151088</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1.200286251054635e-06</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>0.2329683983060217</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.7578485969324917</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.006472001225971314</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.00271100353551532</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>0.9670289604375487</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.02920774981438408</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.000387713941914312</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.003375575806153008</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>0.7079235471749934</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.2108683211041715</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.01648695909144015</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.06472117262939484</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>0.9999999528989951</v>
+      </c>
+      <c r="D56" t="n">
+        <v>5.381573868169038e-11</v>
+      </c>
+      <c r="E56" t="n">
+        <v>4.699692039184996e-08</v>
+      </c>
+      <c r="F56" t="n">
+        <v>5.026875817059759e-11</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>0.2023757944236655</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.05577094903437014</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.0004469870277078885</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.7414062695142564</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>0.9448782423190163</v>
+      </c>
+      <c r="D58" t="n">
+        <v>3.319324153942901e-05</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.03612209607386</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.01896646836558424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Nene audio and changed names
</commit_message>
<xml_diff>
--- a/predict_from_audio/prediction.xlsx
+++ b/predict_from_audio/prediction.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,25 +483,8 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>angry</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0.9999999999999958</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4.291846626024645e-15</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6.66485617840923e-26</v>
-      </c>
-      <c r="F2" t="n">
-        <v>3.548520108061694e-31</v>
+          <t>sm audio</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -516,16 +499,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9999999999948537</v>
+        <v>0.9967240285874112</v>
       </c>
       <c r="D3" t="n">
-        <v>5.146324637887233e-12</v>
+        <v>0.003220225245770692</v>
       </c>
       <c r="E3" t="n">
-        <v>2.810826813893951e-30</v>
+        <v>2.425669507872446e-06</v>
       </c>
       <c r="F3" t="n">
-        <v>5.268669145896358e-29</v>
+        <v>5.332049731042937e-05</v>
       </c>
     </row>
     <row r="4">
@@ -536,20 +519,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.1028777073031261</v>
+        <v>0.9960089464503321</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8529391729352254</v>
+        <v>0.003832517333283918</v>
       </c>
       <c r="E4" t="n">
-        <v>5.034425655902e-10</v>
+        <v>8.938431557726978e-06</v>
       </c>
       <c r="F4" t="n">
-        <v>0.04418311925820596</v>
+        <v>0.0001495977848261474</v>
       </c>
     </row>
     <row r="5">
@@ -560,20 +543,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect happy</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.7666623952473265</v>
+        <v>0.08577395032069544</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2333357142873389</v>
+        <v>0.8899535611938793</v>
       </c>
       <c r="E5" t="n">
-        <v>1.753678623225305e-08</v>
+        <v>0.0003241505332396439</v>
       </c>
       <c r="F5" t="n">
-        <v>1.872928548387014e-06</v>
+        <v>0.02394833795218567</v>
       </c>
     </row>
     <row r="6">
@@ -588,16 +571,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.999999980545106</v>
+        <v>0.9586486044778133</v>
       </c>
       <c r="D6" t="n">
-        <v>1.730659158882568e-08</v>
+        <v>0.04040368563383474</v>
       </c>
       <c r="E6" t="n">
-        <v>4.379235247356553e-16</v>
+        <v>0.0001438221540094927</v>
       </c>
       <c r="F6" t="n">
-        <v>2.148301860307265e-09</v>
+        <v>0.0008038877343422925</v>
       </c>
     </row>
     <row r="7">
@@ -612,22 +595,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.9990268282978271</v>
       </c>
       <c r="D7" t="n">
-        <v>1.924163704260329e-17</v>
+        <v>0.0007856663452184859</v>
       </c>
       <c r="E7" t="n">
-        <v>2.294331200125262e-25</v>
+        <v>1.207733057905328e-06</v>
       </c>
       <c r="F7" t="n">
-        <v>2.205737654997553e-20</v>
+        <v>0.0001862976238963246</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -636,16 +619,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7.160066741041603e-05</v>
+        <v>0.9999764553575379</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9938370957247582</v>
+        <v>1.567219664606199e-05</v>
       </c>
       <c r="E8" t="n">
-        <v>4.655726129925718e-12</v>
+        <v>2.881859564132323e-07</v>
       </c>
       <c r="F8" t="n">
-        <v>0.006091303603175372</v>
+        <v>7.584259859330055e-06</v>
       </c>
     </row>
     <row r="9">
@@ -660,16 +643,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>7.767771464208086e-11</v>
+        <v>8.416545284344562e-05</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9998186783651475</v>
+        <v>0.9971188092388492</v>
       </c>
       <c r="E9" t="n">
-        <v>3.704340991320492e-10</v>
+        <v>4.820323428585023e-06</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0001813211867407489</v>
+        <v>0.002792204984878705</v>
       </c>
     </row>
     <row r="10">
@@ -684,16 +667,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0002001987242701397</v>
+        <v>0.005682913107010259</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9997988591267064</v>
+        <v>0.9096998249575433</v>
       </c>
       <c r="E10" t="n">
-        <v>3.891104573591962e-10</v>
+        <v>0.0002141563827855265</v>
       </c>
       <c r="F10" t="n">
-        <v>9.417599129913047e-07</v>
+        <v>0.08440310555266109</v>
       </c>
     </row>
     <row r="11">
@@ -708,16 +691,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.285877384671724e-05</v>
+        <v>0.002891622294720282</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9998972816141034</v>
+        <v>0.9966465559864562</v>
       </c>
       <c r="E11" t="n">
-        <v>6.163826617593398e-11</v>
+        <v>4.933817120008135e-06</v>
       </c>
       <c r="F11" t="n">
-        <v>2.985955041153062e-05</v>
+        <v>0.0004568879017032881</v>
       </c>
     </row>
     <row r="12">
@@ -732,16 +715,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0001941658518078025</v>
+        <v>0.0007421303237597793</v>
       </c>
       <c r="D12" t="n">
-        <v>0.885309060400899</v>
+        <v>0.9988407208362943</v>
       </c>
       <c r="E12" t="n">
-        <v>8.211051501150986e-10</v>
+        <v>1.569839431807567e-05</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1144967729261881</v>
+        <v>0.0004014504456276824</v>
       </c>
     </row>
     <row r="13">
@@ -756,22 +739,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.001205930314508531</v>
+        <v>0.004507817550229914</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9987940151248954</v>
+        <v>0.9478133902805241</v>
       </c>
       <c r="E13" t="n">
-        <v>5.321840327646175e-08</v>
+        <v>1.678318757113478e-05</v>
       </c>
       <c r="F13" t="n">
-        <v>1.342192599378953e-09</v>
+        <v>0.04766200898167482</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -780,16 +763,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3.655757449281229e-08</v>
+        <v>0.0224334420656406</v>
       </c>
       <c r="D14" t="n">
-        <v>2.577855951990804e-10</v>
+        <v>0.9766381995450102</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9999124400639006</v>
+        <v>0.0001020607900995321</v>
       </c>
       <c r="F14" t="n">
-        <v>8.752312073935968e-05</v>
+        <v>0.0008262975992495603</v>
       </c>
     </row>
     <row r="15">
@@ -804,16 +787,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.972498185852568e-13</v>
+        <v>0.0001774797114995922</v>
       </c>
       <c r="D15" t="n">
-        <v>7.483698164820451e-13</v>
+        <v>0.0001148224023359418</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9999999926922711</v>
+        <v>0.9988502155332722</v>
       </c>
       <c r="F15" t="n">
-        <v>7.306683212888786e-09</v>
+        <v>0.0008574823528922473</v>
       </c>
     </row>
     <row r="16">
@@ -828,16 +811,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1.818326810761002e-09</v>
+        <v>4.225999714959673e-06</v>
       </c>
       <c r="D16" t="n">
-        <v>1.88864279690199e-07</v>
+        <v>2.636248294333487e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9999789101249372</v>
+        <v>0.9999279238767704</v>
       </c>
       <c r="F16" t="n">
-        <v>2.089919245621273e-05</v>
+        <v>4.148764057093747e-05</v>
       </c>
     </row>
     <row r="17">
@@ -852,16 +835,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.0006363943832354439</v>
+        <v>0.004199071164081437</v>
       </c>
       <c r="D17" t="n">
-        <v>5.097935127992823e-07</v>
+        <v>0.0008813746957617593</v>
       </c>
       <c r="E17" t="n">
-        <v>0.7139565301732967</v>
+        <v>0.8967228513443172</v>
       </c>
       <c r="F17" t="n">
-        <v>0.285406565649955</v>
+        <v>0.09819670279583971</v>
       </c>
     </row>
     <row r="18">
@@ -872,20 +855,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect sad</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.0003172675327794079</v>
+        <v>0.2098295926211494</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0001624648103621018</v>
+        <v>0.002349891030542739</v>
       </c>
       <c r="E18" t="n">
-        <v>0.04522183670170381</v>
+        <v>0.00344875127626371</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9542984309551547</v>
+        <v>0.7843717650720441</v>
       </c>
     </row>
     <row r="19">
@@ -896,20 +879,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect happy</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>5.545264395613459e-28</v>
+        <v>0.05484201887834616</v>
       </c>
       <c r="D19" t="n">
-        <v>1.463972414254795e-19</v>
+        <v>0.8036199365179976</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0.006169015935868727</v>
       </c>
       <c r="F19" t="n">
-        <v>3.175274972802759e-27</v>
+        <v>0.1353690286677875</v>
       </c>
     </row>
     <row r="20">
@@ -920,44 +903,44 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.002231696413647554</v>
+        <v>3.041055835125255e-06</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9974179285381959</v>
+        <v>9.672286546408705e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>5.738162865051805e-08</v>
+        <v>0.9999678921650313</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0003503176665278402</v>
+        <v>1.939449258726316e-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect happy</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.385949559080319e-11</v>
+        <v>0.312297503077999</v>
       </c>
       <c r="D21" t="n">
-        <v>2.655396857779116e-06</v>
+        <v>0.6288431530745237</v>
       </c>
       <c r="E21" t="n">
-        <v>1.321731641938074e-13</v>
+        <v>0.0004342219686435462</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9999973445891506</v>
+        <v>0.05842512187883404</v>
       </c>
     </row>
     <row r="22">
@@ -972,16 +955,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.754139667201018e-08</v>
+        <v>0.0005259545986728333</v>
       </c>
       <c r="D22" t="n">
-        <v>2.950762397383278e-09</v>
+        <v>0.004625665039814776</v>
       </c>
       <c r="E22" t="n">
-        <v>7.758754129680849e-08</v>
+        <v>5.107922906874856e-06</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9999998919202996</v>
+        <v>0.9948432724386058</v>
       </c>
     </row>
     <row r="23">
@@ -996,16 +979,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>7.933802066873205e-08</v>
+        <v>0.0001267455517479158</v>
       </c>
       <c r="D23" t="n">
-        <v>2.964548334569894e-06</v>
+        <v>1.229200020561608e-05</v>
       </c>
       <c r="E23" t="n">
-        <v>0.002664593551422074</v>
+        <v>2.797522880316338e-05</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9973323625622228</v>
+        <v>0.9998329872192437</v>
       </c>
     </row>
     <row r="24">
@@ -1020,16 +1003,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.001097362606637019</v>
+        <v>0.0002577775657305929</v>
       </c>
       <c r="D24" t="n">
-        <v>5.848605007532611e-06</v>
+        <v>0.0006762489571278473</v>
       </c>
       <c r="E24" t="n">
-        <v>1.842473284582486e-07</v>
+        <v>2.966577095318264e-05</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9988966045410269</v>
+        <v>0.9990363077061881</v>
       </c>
     </row>
     <row r="25">
@@ -1044,16 +1027,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.00227936324341661</v>
+        <v>0.002481680810421572</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0006771221581906856</v>
+        <v>0.000818218722816309</v>
       </c>
       <c r="E25" t="n">
-        <v>1.563432639650271e-10</v>
+        <v>5.466276960582574e-05</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9970435144420494</v>
+        <v>0.9966454376971562</v>
       </c>
     </row>
     <row r="26">
@@ -1068,22 +1051,22 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1.059517386278515e-08</v>
+        <v>0.002986066824968685</v>
       </c>
       <c r="D26" t="n">
-        <v>0.001041190368569997</v>
+        <v>0.0001710536483409428</v>
       </c>
       <c r="E26" t="n">
-        <v>3.398141903940196e-05</v>
+        <v>7.783942830851323e-06</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9989248176172167</v>
+        <v>0.9968350955838595</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>angry</t>
+          <t>sad</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1092,190 +1075,173 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.9995721705358902</v>
+        <v>0.009244555823201535</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0004277053458163146</v>
+        <v>0.000456278199524126</v>
       </c>
       <c r="E27" t="n">
-        <v>1.240794930920694e-07</v>
+        <v>0.003416993829625012</v>
       </c>
       <c r="F27" t="n">
-        <v>3.880033353820926e-11</v>
+        <v>0.9868821721476492</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>angry</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>0.9999990763143342</v>
-      </c>
-      <c r="D28" t="n">
-        <v>9.206551458264538e-07</v>
-      </c>
-      <c r="E28" t="n">
-        <v>2.895861708235209e-09</v>
-      </c>
-      <c r="F28" t="n">
-        <v>1.346580551683429e-10</v>
+          <t>Nene audio</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.9987928457965177</v>
+        <v>0.5252083611687827</v>
       </c>
       <c r="D29" t="n">
-        <v>0.001131363067335202</v>
+        <v>0.01169757042513848</v>
       </c>
       <c r="E29" t="n">
-        <v>7.52820697739485e-05</v>
+        <v>0.4475445669398703</v>
       </c>
       <c r="F29" t="n">
-        <v>5.090663732402273e-07</v>
+        <v>0.0155495014662084</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.007409017009692965</v>
+        <v>0.2200298905558317</v>
       </c>
       <c r="D30" t="n">
-        <v>0.03906467134675482</v>
+        <v>0.101210001712699</v>
       </c>
       <c r="E30" t="n">
-        <v>0.02094113254565224</v>
+        <v>0.5893830642345245</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9325851790979</v>
+        <v>0.08937704349694479</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1.886445523589289e-08</v>
+        <v>0.08241477764283686</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0727366312636923</v>
+        <v>0.005286091796481958</v>
       </c>
       <c r="E31" t="n">
-        <v>0.6959178584831803</v>
+        <v>0.8603999230227346</v>
       </c>
       <c r="F31" t="n">
-        <v>0.2313454913886721</v>
+        <v>0.05189920753794647</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.959734283109663</v>
+        <v>0.07999333352514325</v>
       </c>
       <c r="D32" t="n">
-        <v>0.03464889177353165</v>
+        <v>0.002519684698830738</v>
       </c>
       <c r="E32" t="n">
-        <v>0.001456493974241639</v>
+        <v>0.5311964953070227</v>
       </c>
       <c r="F32" t="n">
-        <v>0.004160331142563724</v>
+        <v>0.3862904864690033</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>7.661429068461271e-05</v>
+        <v>0.03128695845425549</v>
       </c>
       <c r="D33" t="n">
-        <v>0.006508287310060995</v>
+        <v>0.05536497610654026</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9923101257946085</v>
+        <v>0.6931961473686689</v>
       </c>
       <c r="F33" t="n">
-        <v>0.001104972604645775</v>
+        <v>0.2201519180705354</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.271436182264907e-09</v>
+        <v>0.01830820044170853</v>
       </c>
       <c r="D34" t="n">
-        <v>0.006220614286581693</v>
+        <v>0.9472362203938731</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9902612076977917</v>
+        <v>0.03198046260907238</v>
       </c>
       <c r="F34" t="n">
-        <v>0.00351817674419033</v>
+        <v>0.002475116555346005</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>angry</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1284,70 +1250,70 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.9999981530185628</v>
+        <v>0.008346901562856585</v>
       </c>
       <c r="D35" t="n">
-        <v>5.841941782252971e-07</v>
+        <v>0.04005478956598563</v>
       </c>
       <c r="E35" t="n">
-        <v>1.271615089490744e-09</v>
+        <v>0.8991061857580188</v>
       </c>
       <c r="F35" t="n">
-        <v>1.261515643896474e-06</v>
+        <v>0.05249212311313895</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>angry</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect happy</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.9539258530745879</v>
+        <v>0.1163675564131164</v>
       </c>
       <c r="D36" t="n">
-        <v>0.04607403663865661</v>
+        <v>0.3327085892734508</v>
       </c>
       <c r="E36" t="n">
-        <v>2.526945979541792e-11</v>
+        <v>0.2814794358748977</v>
       </c>
       <c r="F36" t="n">
-        <v>1.102614859899988e-07</v>
+        <v>0.269444418438535</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1.5981035990305e-08</v>
+        <v>0.003780696404286505</v>
       </c>
       <c r="D37" t="n">
-        <v>0.008761163441396354</v>
+        <v>0.00684330791479671</v>
       </c>
       <c r="E37" t="n">
-        <v>1.242975578146528e-06</v>
+        <v>0.9705000095819848</v>
       </c>
       <c r="F37" t="n">
-        <v>0.9912375776019895</v>
+        <v>0.01887598609893204</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1356,16 +1322,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.004799249855495546</v>
+        <v>0.0013306929041822</v>
       </c>
       <c r="D38" t="n">
-        <v>0.9817976558239718</v>
+        <v>0.003026269862183079</v>
       </c>
       <c r="E38" t="n">
-        <v>6.438453634667692e-05</v>
+        <v>0.9900756411769762</v>
       </c>
       <c r="F38" t="n">
-        <v>0.01333870978418593</v>
+        <v>0.005567396056658348</v>
       </c>
     </row>
     <row r="39">
@@ -1380,40 +1346,40 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.001534786125160449</v>
+        <v>0.0006092153589533754</v>
       </c>
       <c r="D39" t="n">
-        <v>0.3044128215254032</v>
+        <v>0.0006195691362252042</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5033205107084728</v>
+        <v>0.9961504076175897</v>
       </c>
       <c r="F39" t="n">
-        <v>0.1907318816409633</v>
+        <v>0.002620807887231779</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>sad</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1.313337767115214e-05</v>
+        <v>0.0004418266400282933</v>
       </c>
       <c r="D40" t="n">
-        <v>0.7244059500682311</v>
+        <v>0.0006679984600360786</v>
       </c>
       <c r="E40" t="n">
-        <v>0.2507082737100196</v>
+        <v>0.9771924215599076</v>
       </c>
       <c r="F40" t="n">
-        <v>0.02487264284407821</v>
+        <v>0.02169775334002799</v>
       </c>
     </row>
     <row r="41">
@@ -1424,20 +1390,20 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.0001853635227671776</v>
+        <v>0.008753485939823181</v>
       </c>
       <c r="D41" t="n">
-        <v>0.595294055793272</v>
+        <v>0.02262280284392373</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0761799787898487</v>
+        <v>0.9334776679379098</v>
       </c>
       <c r="F41" t="n">
-        <v>0.3283406018941121</v>
+        <v>0.03514604327834329</v>
       </c>
     </row>
     <row r="42">
@@ -1448,44 +1414,27 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.1403318805639651</v>
+        <v>0.001521355343825038</v>
       </c>
       <c r="D42" t="n">
-        <v>0.1233044973016834</v>
+        <v>0.01092431702400422</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5957044938677239</v>
+        <v>0.9694618908996385</v>
       </c>
       <c r="F42" t="n">
-        <v>0.1406591282666275</v>
+        <v>0.01809243673253225</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>angry</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>incorrect</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
-        <v>0.007871794831014104</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0.6128756203690255</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0.00011859168776166</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0.3791339931121985</v>
+          <t>JLCorpus audio</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -1500,160 +1449,160 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.933342097924862</v>
+        <v>0.8249788368708426</v>
       </c>
       <c r="D44" t="n">
-        <v>0.06404864795599134</v>
+        <v>0.1529362846963662</v>
       </c>
       <c r="E44" t="n">
-        <v>1.469181154394465e-05</v>
+        <v>0.002166296612103928</v>
       </c>
       <c r="F44" t="n">
-        <v>0.002594562307602802</v>
+        <v>0.01991858182068736</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.9999339846265671</v>
+        <v>0.8843187131788993</v>
       </c>
       <c r="D45" t="n">
-        <v>3.391343729260749e-05</v>
+        <v>0.1014817834432492</v>
       </c>
       <c r="E45" t="n">
-        <v>3.098749641246511e-05</v>
+        <v>0.007704776759221276</v>
       </c>
       <c r="F45" t="n">
-        <v>1.114439727982079e-06</v>
+        <v>0.006494726618630115</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.9815260565074053</v>
+        <v>0.8578108046517005</v>
       </c>
       <c r="D46" t="n">
-        <v>0.01842195184277194</v>
+        <v>0.1050031881631763</v>
       </c>
       <c r="E46" t="n">
-        <v>1.301744078155718e-05</v>
+        <v>0.0009784896407430868</v>
       </c>
       <c r="F46" t="n">
-        <v>3.897420904106367e-05</v>
+        <v>0.03620751754438008</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>6.834589457218006e-05</v>
+        <v>0.6274666990069644</v>
       </c>
       <c r="D47" t="n">
-        <v>3.18409901194095e-07</v>
+        <v>0.1538673711567887</v>
       </c>
       <c r="E47" t="n">
-        <v>0.000173686538987348</v>
+        <v>0.006910498976568267</v>
       </c>
       <c r="F47" t="n">
-        <v>0.9997576491565392</v>
+        <v>0.2117554308596787</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect happy</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.00112738871308322</v>
+        <v>0.3117819229374159</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0006072808962604886</v>
+        <v>0.4168391432605447</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0001837692321294081</v>
+        <v>0.1550668591685605</v>
       </c>
       <c r="F48" t="n">
-        <v>0.998081561158527</v>
+        <v>0.1163120746334789</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.0448076378585431</v>
+        <v>0.1583807188532174</v>
       </c>
       <c r="D49" t="n">
-        <v>0.01209983737535265</v>
+        <v>0.06246181992863134</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0004834905551472906</v>
+        <v>0.7489639394922224</v>
       </c>
       <c r="F49" t="n">
-        <v>0.942609034210957</v>
+        <v>0.03019352172592871</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>angry</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.8336064826098039</v>
+        <v>0.2424609054089119</v>
       </c>
       <c r="D50" t="n">
-        <v>0.1505400630220914</v>
+        <v>0.009339445285462137</v>
       </c>
       <c r="E50" t="n">
-        <v>0.0001059544595925266</v>
+        <v>0.7462358050047575</v>
       </c>
       <c r="F50" t="n">
-        <v>0.01574749990851225</v>
+        <v>0.001963844300868374</v>
       </c>
     </row>
     <row r="51">
@@ -1664,44 +1613,44 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect happy</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>6.551771406901146e-07</v>
+        <v>0.06660464081370406</v>
       </c>
       <c r="D51" t="n">
-        <v>1.356957952646745e-09</v>
+        <v>0.6675463582039703</v>
       </c>
       <c r="E51" t="n">
-        <v>0.9999993434657899</v>
+        <v>0.186910313358817</v>
       </c>
       <c r="F51" t="n">
-        <v>1.113762560245061e-13</v>
+        <v>0.07893868762350853</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>angry</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.2332444467004595</v>
+        <v>0.08491507685580395</v>
       </c>
       <c r="D52" t="n">
-        <v>0.0003675825981806465</v>
+        <v>0.7141561784102907</v>
       </c>
       <c r="E52" t="n">
-        <v>0.7663867704151088</v>
+        <v>0.01873309311383283</v>
       </c>
       <c r="F52" t="n">
-        <v>1.200286251054635e-06</v>
+        <v>0.1821956516200726</v>
       </c>
     </row>
     <row r="53">
@@ -1712,20 +1661,20 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect sad</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.2329683983060217</v>
+        <v>0.003429546761011103</v>
       </c>
       <c r="D53" t="n">
-        <v>0.7578485969324917</v>
+        <v>0.01370493462987036</v>
       </c>
       <c r="E53" t="n">
-        <v>0.006472001225971314</v>
+        <v>0.006891811167023417</v>
       </c>
       <c r="F53" t="n">
-        <v>0.00271100353551532</v>
+        <v>0.9759737074420952</v>
       </c>
     </row>
     <row r="54">
@@ -1736,116 +1685,524 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect sad</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.9670289604375487</v>
+        <v>0.02579026200145208</v>
       </c>
       <c r="D54" t="n">
-        <v>0.02920774981438408</v>
+        <v>0.1527715714886227</v>
       </c>
       <c r="E54" t="n">
-        <v>0.000387713941914312</v>
+        <v>0.002452411207204725</v>
       </c>
       <c r="F54" t="n">
-        <v>0.003375575806153008</v>
+        <v>0.8189857553027204</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect sad</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.7079235471749934</v>
+        <v>0.01331914036319754</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2108683211041715</v>
+        <v>0.05464932477184229</v>
       </c>
       <c r="E55" t="n">
-        <v>0.01648695909144015</v>
+        <v>0.0008830306206513766</v>
       </c>
       <c r="F55" t="n">
-        <v>0.06472117262939484</v>
+        <v>0.9311485042443088</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>incorrect</t>
+          <t>incorrect angry</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.9999999528989951</v>
+        <v>0.9970876419481446</v>
       </c>
       <c r="D56" t="n">
-        <v>5.381573868169038e-11</v>
+        <v>7.017074963211012e-05</v>
       </c>
       <c r="E56" t="n">
-        <v>4.699692039184996e-08</v>
+        <v>0.0001335010119803655</v>
       </c>
       <c r="F56" t="n">
-        <v>5.026875817059759e-11</v>
+        <v>0.002708686290243477</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect sad</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.2023757944236655</v>
+        <v>0.08126454008679292</v>
       </c>
       <c r="D57" t="n">
-        <v>0.05577094903437014</v>
+        <v>0.3479009519734195</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0004469870277078885</v>
+        <v>0.004147636301056327</v>
       </c>
       <c r="F57" t="n">
-        <v>0.7414062695142564</v>
+        <v>0.5666868716387313</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>incorrect neutral</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>0.0009411322230673107</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.009887117660395617</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.9752196307049895</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.01395211941154751</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>incorrect neutral</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>0.0380987585695971</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.01721955437805785</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.8074667343925427</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.1372149526598023</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>incorrect sad</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>0.1847767740949373</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.1306790823700288</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.1563318774753384</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.5282122660596955</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>0.04982068825045143</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.2090051449685728</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.474815521680839</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.2663586451001371</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>0.01788202162282966</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.08336170971836368</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.4527089885261286</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.446047280132678</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>incorrect sad</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0.002342730038518375</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.01874987990457705</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.3634789464963444</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.6154284435605601</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>incorrect sad</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>0.01088158857862999</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.03298322623575701</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.1063184136629956</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.8498167715226175</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>0.01021158700357143</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.00458337362136785</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.6128418243999014</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.3723632149751593</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>incorrect sad</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>0.03283825418528316</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.01370644943371203</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.4484489753463254</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.5050063210346794</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>incorrect sad</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0.02092377406254374</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.01749718974694352</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.1628495858141605</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.7987294503763522</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
           <t>sad</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>incorrect</t>
-        </is>
-      </c>
-      <c r="C58" t="n">
-        <v>0.9448782423190163</v>
-      </c>
-      <c r="D58" t="n">
-        <v>3.319324153942901e-05</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0.03612209607386</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0.01896646836558424</v>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0.002350423950973783</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.007240551165038419</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.06217455800496971</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.9282344668790181</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>incorrect neutral</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0.00243512581224943</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.006175243307718647</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.9415841381569668</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.04980549272306525</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0.002168757091693651</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.009806424037568292</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.4219450085658258</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.5660798103049124</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>0.007934648959867898</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.003976951620888842</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.01544076505138055</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.9726476343678627</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>incorrect happy</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>0.1022201755587806</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.3474953829640091</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.2207682530560133</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.3295161884211967</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>0.002980680037855231</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.01521446713556014</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.1777813637693905</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.8040234890571942</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0.004492317114871837</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.007266246629477249</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.3727510209706461</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.6154904152850047</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0.002504843191026519</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.007721362889234841</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.04585785055999618</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.9439159433597424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trained with new data and improved prediction
</commit_message>
<xml_diff>
--- a/predict_from_audio/prediction.xlsx
+++ b/predict_from_audio/prediction.xlsx
@@ -499,16 +499,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9967240285874112</v>
+        <v>0.9999999980980918</v>
       </c>
       <c r="D3" t="n">
-        <v>0.003220225245770692</v>
+        <v>1.901908152575907e-09</v>
       </c>
       <c r="E3" t="n">
-        <v>2.425669507872446e-06</v>
+        <v>6.241178625482975e-28</v>
       </c>
       <c r="F3" t="n">
-        <v>5.332049731042937e-05</v>
+        <v>3.24068762193153e-26</v>
       </c>
     </row>
     <row r="4">
@@ -523,16 +523,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9960089464503321</v>
+        <v>0.9999999988419648</v>
       </c>
       <c r="D4" t="n">
-        <v>0.003832517333283918</v>
+        <v>1.158035163895001e-09</v>
       </c>
       <c r="E4" t="n">
-        <v>8.938431557726978e-06</v>
+        <v>6.9807208838602e-32</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0001495977848261474</v>
+        <v>9.205529105521453e-28</v>
       </c>
     </row>
     <row r="5">
@@ -547,16 +547,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.08577395032069544</v>
+        <v>0.07978859772950675</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8899535611938793</v>
+        <v>0.915950241603852</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0003241505332396439</v>
+        <v>4.03284255152515e-12</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02394833795218567</v>
+        <v>0.004261160662608308</v>
       </c>
     </row>
     <row r="6">
@@ -571,16 +571,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9586486044778133</v>
+        <v>0.7317215961819231</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04040368563383474</v>
+        <v>0.2682693124181322</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0001438221540094927</v>
+        <v>3.700705271353019e-13</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0008038877343422925</v>
+        <v>9.091399574511182e-06</v>
       </c>
     </row>
     <row r="7">
@@ -595,16 +595,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9990268282978271</v>
+        <v>0.9999998682229498</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0007856663452184859</v>
+        <v>1.317725146248232e-07</v>
       </c>
       <c r="E7" t="n">
-        <v>1.207733057905328e-06</v>
+        <v>3.596490645575583e-18</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0001862976238963246</v>
+        <v>4.535385146185481e-12</v>
       </c>
     </row>
     <row r="8">
@@ -619,16 +619,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9999764553575379</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>1.567219664606199e-05</v>
+        <v>7.247268564707396e-27</v>
       </c>
       <c r="E8" t="n">
-        <v>2.881859564132323e-07</v>
+        <v>1.825553619872027e-28</v>
       </c>
       <c r="F8" t="n">
-        <v>7.584259859330055e-06</v>
+        <v>1.443668456632889e-23</v>
       </c>
     </row>
     <row r="9">
@@ -643,16 +643,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8.416545284344562e-05</v>
+        <v>2.076438624114156e-07</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9971188092388492</v>
+        <v>0.7552214762279843</v>
       </c>
       <c r="E9" t="n">
-        <v>4.820323428585023e-06</v>
+        <v>4.258497450727397e-15</v>
       </c>
       <c r="F9" t="n">
-        <v>0.002792204984878705</v>
+        <v>0.244778316128149</v>
       </c>
     </row>
     <row r="10">
@@ -667,16 +667,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.005682913107010259</v>
+        <v>1.359082569358502e-11</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9096998249575433</v>
+        <v>0.9974690308427606</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0002141563827855265</v>
+        <v>8.168723877804321e-17</v>
       </c>
       <c r="F10" t="n">
-        <v>0.08440310555266109</v>
+        <v>0.00253096914364843</v>
       </c>
     </row>
     <row r="11">
@@ -691,16 +691,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.002891622294720282</v>
+        <v>1.341148972453739e-06</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9966465559864562</v>
+        <v>0.9999986427433988</v>
       </c>
       <c r="E11" t="n">
-        <v>4.933817120008135e-06</v>
+        <v>6.620795969253407e-14</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0004568879017032881</v>
+        <v>1.610756277991192e-08</v>
       </c>
     </row>
     <row r="12">
@@ -715,16 +715,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0007421303237597793</v>
+        <v>8.159915161718975e-05</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9988407208362943</v>
+        <v>0.9998922519320573</v>
       </c>
       <c r="E12" t="n">
-        <v>1.569839431807567e-05</v>
+        <v>1.263083644464787e-18</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0004014504456276824</v>
+        <v>2.614891632553173e-05</v>
       </c>
     </row>
     <row r="13">
@@ -739,16 +739,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.004507817550229914</v>
+        <v>3.611808599893745e-06</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9478133902805241</v>
+        <v>0.9999363203536533</v>
       </c>
       <c r="E13" t="n">
-        <v>1.678318757113478e-05</v>
+        <v>5.290326123811149e-15</v>
       </c>
       <c r="F13" t="n">
-        <v>0.04766200898167482</v>
+        <v>6.006783774129995e-05</v>
       </c>
     </row>
     <row r="14">
@@ -763,16 +763,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.0224334420656406</v>
+        <v>1.136807163704048e-08</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9766381995450102</v>
+        <v>0.9999998836976471</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0001020607900995321</v>
+        <v>1.049342790594607e-07</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0008262975992495603</v>
+        <v>2.213137904753125e-15</v>
       </c>
     </row>
     <row r="15">
@@ -787,16 +787,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.0001774797114995922</v>
+        <v>1.788905429021265e-06</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0001148224023359418</v>
+        <v>2.324239124415401e-07</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9988502155332722</v>
+        <v>0.9989152990127276</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0008574823528922473</v>
+        <v>0.001082679657930955</v>
       </c>
     </row>
     <row r="16">
@@ -811,16 +811,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4.225999714959673e-06</v>
+        <v>4.825020100563713e-13</v>
       </c>
       <c r="D16" t="n">
-        <v>2.636248294333487e-05</v>
+        <v>4.755995081681969e-06</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9999279238767704</v>
+        <v>0.9999925942116565</v>
       </c>
       <c r="F16" t="n">
-        <v>4.148764057093747e-05</v>
+        <v>2.649792779297926e-06</v>
       </c>
     </row>
     <row r="17">
@@ -835,16 +835,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.004199071164081437</v>
+        <v>5.267385917871837e-14</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0008813746957617593</v>
+        <v>5.91386014091039e-14</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8967228513443172</v>
+        <v>0.9999999997338691</v>
       </c>
       <c r="F17" t="n">
-        <v>0.09819670279583971</v>
+        <v>2.660188942789926e-10</v>
       </c>
     </row>
     <row r="18">
@@ -859,16 +859,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.2098295926211494</v>
+        <v>9.167849298109255e-07</v>
       </c>
       <c r="D18" t="n">
-        <v>0.002349891030542739</v>
+        <v>1.380257509500387e-12</v>
       </c>
       <c r="E18" t="n">
-        <v>0.00344875127626371</v>
+        <v>0.2170218620673969</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7843717650720441</v>
+        <v>0.7829772211462931</v>
       </c>
     </row>
     <row r="19">
@@ -879,20 +879,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>incorrect happy</t>
+          <t>incorrect sad</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.05484201887834616</v>
+        <v>0.002521283185271597</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8036199365179976</v>
+        <v>0.0003114556458699814</v>
       </c>
       <c r="E19" t="n">
-        <v>0.006169015935868727</v>
+        <v>1.201146502889526e-05</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1353690286677875</v>
+        <v>0.9971552497038294</v>
       </c>
     </row>
     <row r="20">
@@ -907,16 +907,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3.041055835125255e-06</v>
+        <v>1.627230495322843e-28</v>
       </c>
       <c r="D20" t="n">
-        <v>9.672286546408705e-06</v>
+        <v>1.108152862671469e-15</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9999678921650313</v>
+        <v>0.9999999999999989</v>
       </c>
       <c r="F20" t="n">
-        <v>1.939449258726316e-05</v>
+        <v>4.847583700422469e-24</v>
       </c>
     </row>
     <row r="21">
@@ -931,16 +931,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.312297503077999</v>
+        <v>9.872802888308033e-05</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6288431530745237</v>
+        <v>0.9996306605983805</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0004342219686435462</v>
+        <v>1.88507559351379e-07</v>
       </c>
       <c r="F21" t="n">
-        <v>0.05842512187883404</v>
+        <v>0.0002704228651769976</v>
       </c>
     </row>
     <row r="22">
@@ -955,16 +955,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.0005259545986728333</v>
+        <v>1.043999183178242e-13</v>
       </c>
       <c r="D22" t="n">
-        <v>0.004625665039814776</v>
+        <v>2.563088372874556e-08</v>
       </c>
       <c r="E22" t="n">
-        <v>5.107922906874856e-06</v>
+        <v>1.419079391266617e-17</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9948432724386058</v>
+        <v>0.9999999743690118</v>
       </c>
     </row>
     <row r="23">
@@ -979,16 +979,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.0001267455517479158</v>
+        <v>7.864140492484909e-08</v>
       </c>
       <c r="D23" t="n">
-        <v>1.229200020561608e-05</v>
+        <v>1.207828392708157e-05</v>
       </c>
       <c r="E23" t="n">
-        <v>2.797522880316338e-05</v>
+        <v>8.623856834011515e-10</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9998329872192437</v>
+        <v>0.9999878422122824</v>
       </c>
     </row>
     <row r="24">
@@ -1003,16 +1003,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.0002577775657305929</v>
+        <v>9.441774953955721e-05</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0006762489571278473</v>
+        <v>0.0009011389545672526</v>
       </c>
       <c r="E24" t="n">
-        <v>2.966577095318264e-05</v>
+        <v>1.801610623829556e-06</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9990363077061881</v>
+        <v>0.9990026416852694</v>
       </c>
     </row>
     <row r="25">
@@ -1027,16 +1027,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.002481680810421572</v>
+        <v>0.0005691952652516235</v>
       </c>
       <c r="D25" t="n">
-        <v>0.000818218722816309</v>
+        <v>0.01157272178444115</v>
       </c>
       <c r="E25" t="n">
-        <v>5.466276960582574e-05</v>
+        <v>2.11764463441168e-09</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9966454376971562</v>
+        <v>0.9878580808326626</v>
       </c>
     </row>
     <row r="26">
@@ -1051,16 +1051,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.002986066824968685</v>
+        <v>0.000429987230323094</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0001710536483409428</v>
+        <v>6.171799975852523e-05</v>
       </c>
       <c r="E26" t="n">
-        <v>7.783942830851323e-06</v>
+        <v>3.53057221793778e-16</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9968350955838595</v>
+        <v>0.999508294769918</v>
       </c>
     </row>
     <row r="27">
@@ -1071,20 +1071,20 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.009244555823201535</v>
+        <v>0.0005401609236637914</v>
       </c>
       <c r="D27" t="n">
-        <v>0.000456278199524126</v>
+        <v>0.000198378222293387</v>
       </c>
       <c r="E27" t="n">
-        <v>0.003416993829625012</v>
+        <v>0.9991767897316592</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9868821721476492</v>
+        <v>8.467112238363382e-05</v>
       </c>
     </row>
     <row r="28">
@@ -1102,20 +1102,20 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect happy</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.5252083611687827</v>
+        <v>0.0814425560285887</v>
       </c>
       <c r="D29" t="n">
-        <v>0.01169757042513848</v>
+        <v>0.9185573502682775</v>
       </c>
       <c r="E29" t="n">
-        <v>0.4475445669398703</v>
+        <v>9.370313391330304e-08</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0155495014662084</v>
+        <v>5.309634488989088e-22</v>
       </c>
     </row>
     <row r="30">
@@ -1126,20 +1126,20 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.2200298905558317</v>
+        <v>0.9985732142207621</v>
       </c>
       <c r="D30" t="n">
-        <v>0.101210001712699</v>
+        <v>0.0003990740848488969</v>
       </c>
       <c r="E30" t="n">
-        <v>0.5893830642345245</v>
+        <v>0.001025864727617267</v>
       </c>
       <c r="F30" t="n">
-        <v>0.08937704349694479</v>
+        <v>1.846966771687364e-06</v>
       </c>
     </row>
     <row r="31">
@@ -1154,16 +1154,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.08241477764283686</v>
+        <v>0.01288722464345116</v>
       </c>
       <c r="D31" t="n">
-        <v>0.005286091796481958</v>
+        <v>0.0002606971997256433</v>
       </c>
       <c r="E31" t="n">
-        <v>0.8603999230227346</v>
+        <v>0.9868520781567823</v>
       </c>
       <c r="F31" t="n">
-        <v>0.05189920753794647</v>
+        <v>4.065066838881868e-14</v>
       </c>
     </row>
     <row r="32">
@@ -1174,20 +1174,20 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.07999333352514325</v>
+        <v>1.426009818619849e-09</v>
       </c>
       <c r="D32" t="n">
-        <v>0.002519684698830738</v>
+        <v>0.8896752896596947</v>
       </c>
       <c r="E32" t="n">
-        <v>0.5311964953070227</v>
+        <v>0.0001206871018144671</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3862904864690033</v>
+        <v>0.1102040218124811</v>
       </c>
     </row>
     <row r="33">
@@ -1202,16 +1202,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.03128695845425549</v>
+        <v>3.503649579178466e-05</v>
       </c>
       <c r="D33" t="n">
-        <v>0.05536497610654026</v>
+        <v>0.0347793659543468</v>
       </c>
       <c r="E33" t="n">
-        <v>0.6931961473686689</v>
+        <v>0.9651773564297866</v>
       </c>
       <c r="F33" t="n">
-        <v>0.2201519180705354</v>
+        <v>8.241120074756249e-06</v>
       </c>
     </row>
     <row r="34">
@@ -1226,16 +1226,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.01830820044170853</v>
+        <v>4.014697095164784e-05</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9472362203938731</v>
+        <v>0.9986293315232968</v>
       </c>
       <c r="E34" t="n">
-        <v>0.03198046260907238</v>
+        <v>0.001330520708528741</v>
       </c>
       <c r="F34" t="n">
-        <v>0.002475116555346005</v>
+        <v>7.972228314141262e-10</v>
       </c>
     </row>
     <row r="35">
@@ -1250,16 +1250,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.008346901562856585</v>
+        <v>1.943800064090439e-08</v>
       </c>
       <c r="D35" t="n">
-        <v>0.04005478956598563</v>
+        <v>4.086935124253035e-07</v>
       </c>
       <c r="E35" t="n">
-        <v>0.8991061857580188</v>
+        <v>0.9999995714443086</v>
       </c>
       <c r="F35" t="n">
-        <v>0.05249212311313895</v>
+        <v>4.241783356967995e-10</v>
       </c>
     </row>
     <row r="36">
@@ -1270,20 +1270,20 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>incorrect happy</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.1163675564131164</v>
+        <v>1.403596674930701e-09</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3327085892734508</v>
+        <v>1.185880567598732e-06</v>
       </c>
       <c r="E36" t="n">
-        <v>0.2814794358748977</v>
+        <v>0.9999873566523821</v>
       </c>
       <c r="F36" t="n">
-        <v>0.269444418438535</v>
+        <v>1.145606345365589e-05</v>
       </c>
     </row>
     <row r="37">
@@ -1298,16 +1298,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.003780696404286505</v>
+        <v>1.226635068154167e-11</v>
       </c>
       <c r="D37" t="n">
-        <v>0.00684330791479671</v>
+        <v>4.884522802381617e-09</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9705000095819848</v>
+        <v>0.9999999942280866</v>
       </c>
       <c r="F37" t="n">
-        <v>0.01887598609893204</v>
+        <v>8.751242892619664e-10</v>
       </c>
     </row>
     <row r="38">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.0013306929041822</v>
+        <v>4.306242226912951e-10</v>
       </c>
       <c r="D38" t="n">
-        <v>0.003026269862183079</v>
+        <v>1.777426296487112e-09</v>
       </c>
       <c r="E38" t="n">
-        <v>0.9900756411769762</v>
+        <v>0.9999999961169554</v>
       </c>
       <c r="F38" t="n">
-        <v>0.005567396056658348</v>
+        <v>1.674993918355791e-09</v>
       </c>
     </row>
     <row r="39">
@@ -1346,16 +1346,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.0006092153589533754</v>
+        <v>1.208491988796428e-12</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0006195691362252042</v>
+        <v>9.4144957652019e-11</v>
       </c>
       <c r="E39" t="n">
-        <v>0.9961504076175897</v>
+        <v>0.9999999998804396</v>
       </c>
       <c r="F39" t="n">
-        <v>0.002620807887231779</v>
+        <v>2.420687821437202e-11</v>
       </c>
     </row>
     <row r="40">
@@ -1370,16 +1370,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.0004418266400282933</v>
+        <v>6.734878510948267e-14</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0006679984600360786</v>
+        <v>9.296465752113463e-10</v>
       </c>
       <c r="E40" t="n">
-        <v>0.9771924215599076</v>
+        <v>0.9999999990700406</v>
       </c>
       <c r="F40" t="n">
-        <v>0.02169775334002799</v>
+        <v>2.454941920588478e-13</v>
       </c>
     </row>
     <row r="41">
@@ -1394,16 +1394,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.008753485939823181</v>
+        <v>1.291918655052882e-09</v>
       </c>
       <c r="D41" t="n">
-        <v>0.02262280284392373</v>
+        <v>0.0008702119792345535</v>
       </c>
       <c r="E41" t="n">
-        <v>0.9334776679379098</v>
+        <v>0.9962375563123423</v>
       </c>
       <c r="F41" t="n">
-        <v>0.03514604327834329</v>
+        <v>0.002892230416504446</v>
       </c>
     </row>
     <row r="42">
@@ -1414,20 +1414,20 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.001521355343825038</v>
+        <v>1.776056614694799e-14</v>
       </c>
       <c r="D42" t="n">
-        <v>0.01092431702400422</v>
+        <v>8.252562008742703e-12</v>
       </c>
       <c r="E42" t="n">
-        <v>0.9694618908996385</v>
+        <v>0.009795382846568869</v>
       </c>
       <c r="F42" t="n">
-        <v>0.01809243673253225</v>
+        <v>0.9902046171451608</v>
       </c>
     </row>
     <row r="43">
@@ -1445,20 +1445,20 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect happy</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.8249788368708426</v>
+        <v>0.03130013732308146</v>
       </c>
       <c r="D44" t="n">
-        <v>0.1529362846963662</v>
+        <v>0.9686998321688762</v>
       </c>
       <c r="E44" t="n">
-        <v>0.002166296612103928</v>
+        <v>2.73405502151761e-08</v>
       </c>
       <c r="F44" t="n">
-        <v>0.01991858182068736</v>
+        <v>3.167491882656891e-09</v>
       </c>
     </row>
     <row r="45">
@@ -1473,16 +1473,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.8843187131788993</v>
+        <v>0.9999997658712945</v>
       </c>
       <c r="D45" t="n">
-        <v>0.1014817834432492</v>
+        <v>2.341253064950237e-07</v>
       </c>
       <c r="E45" t="n">
-        <v>0.007704776759221276</v>
+        <v>3.393911730012946e-12</v>
       </c>
       <c r="F45" t="n">
-        <v>0.006494726618630115</v>
+        <v>5.170900987975009e-15</v>
       </c>
     </row>
     <row r="46">
@@ -1497,16 +1497,16 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.8578108046517005</v>
+        <v>0.9999999827512297</v>
       </c>
       <c r="D46" t="n">
-        <v>0.1050031881631763</v>
+        <v>1.724808539883253e-08</v>
       </c>
       <c r="E46" t="n">
-        <v>0.0009784896407430868</v>
+        <v>9.051866816753053e-16</v>
       </c>
       <c r="F46" t="n">
-        <v>0.03620751754438008</v>
+        <v>6.841270024694351e-13</v>
       </c>
     </row>
     <row r="47">
@@ -1521,16 +1521,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.6274666990069644</v>
+        <v>0.9999981489460259</v>
       </c>
       <c r="D47" t="n">
-        <v>0.1538673711567887</v>
+        <v>1.805580582609897e-06</v>
       </c>
       <c r="E47" t="n">
-        <v>0.006910498976568267</v>
+        <v>4.525431365029557e-08</v>
       </c>
       <c r="F47" t="n">
-        <v>0.2117554308596787</v>
+        <v>2.190778614993478e-10</v>
       </c>
     </row>
     <row r="48">
@@ -1545,16 +1545,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.3117819229374159</v>
+        <v>0.3618318166648764</v>
       </c>
       <c r="D48" t="n">
-        <v>0.4168391432605447</v>
+        <v>0.6381647473595103</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1550668591685605</v>
+        <v>2.887581689093385e-08</v>
       </c>
       <c r="F48" t="n">
-        <v>0.1163120746334789</v>
+        <v>3.407099796163236e-06</v>
       </c>
     </row>
     <row r="49">
@@ -1565,20 +1565,20 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.1583807188532174</v>
+        <v>0.6473000818358808</v>
       </c>
       <c r="D49" t="n">
-        <v>0.06246181992863134</v>
+        <v>0.3526649760793807</v>
       </c>
       <c r="E49" t="n">
-        <v>0.7489639394922224</v>
+        <v>3.421235727185909e-05</v>
       </c>
       <c r="F49" t="n">
-        <v>0.03019352172592871</v>
+        <v>7.297274665193926e-07</v>
       </c>
     </row>
     <row r="50">
@@ -1589,20 +1589,20 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.2424609054089119</v>
+        <v>0.9999999910402405</v>
       </c>
       <c r="D50" t="n">
-        <v>0.009339445285462137</v>
+        <v>8.959626294145054e-09</v>
       </c>
       <c r="E50" t="n">
-        <v>0.7462358050047575</v>
+        <v>1.333085419509235e-13</v>
       </c>
       <c r="F50" t="n">
-        <v>0.001963844300868374</v>
+        <v>1.985225483841853e-18</v>
       </c>
     </row>
     <row r="51">
@@ -1613,20 +1613,20 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>incorrect happy</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.06660464081370406</v>
+        <v>0.9999999988311012</v>
       </c>
       <c r="D51" t="n">
-        <v>0.6675463582039703</v>
+        <v>1.031173686272702e-09</v>
       </c>
       <c r="E51" t="n">
-        <v>0.186910313358817</v>
+        <v>1.113750939167807e-10</v>
       </c>
       <c r="F51" t="n">
-        <v>0.07893868762350853</v>
+        <v>2.635010776557755e-11</v>
       </c>
     </row>
     <row r="52">
@@ -1641,16 +1641,16 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.08491507685580395</v>
+        <v>0.02352517099769824</v>
       </c>
       <c r="D52" t="n">
-        <v>0.7141561784102907</v>
+        <v>0.8052797136071453</v>
       </c>
       <c r="E52" t="n">
-        <v>0.01873309311383283</v>
+        <v>0.1711946884165533</v>
       </c>
       <c r="F52" t="n">
-        <v>0.1821956516200726</v>
+        <v>4.269786029598599e-07</v>
       </c>
     </row>
     <row r="53">
@@ -1661,20 +1661,20 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.003429546761011103</v>
+        <v>0.0003463828112435817</v>
       </c>
       <c r="D53" t="n">
-        <v>0.01370493462987036</v>
+        <v>0.9992461016441622</v>
       </c>
       <c r="E53" t="n">
-        <v>0.006891811167023417</v>
+        <v>0.0003926137395219223</v>
       </c>
       <c r="F53" t="n">
-        <v>0.9759737074420952</v>
+        <v>1.490180507246497e-05</v>
       </c>
     </row>
     <row r="54">
@@ -1685,20 +1685,20 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.02579026200145208</v>
+        <v>2.123060364492161e-07</v>
       </c>
       <c r="D54" t="n">
-        <v>0.1527715714886227</v>
+        <v>0.9999997812632376</v>
       </c>
       <c r="E54" t="n">
-        <v>0.002452411207204725</v>
+        <v>6.405090017418388e-09</v>
       </c>
       <c r="F54" t="n">
-        <v>0.8189857553027204</v>
+        <v>2.563597522620052e-11</v>
       </c>
     </row>
     <row r="55">
@@ -1709,20 +1709,20 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.01331914036319754</v>
+        <v>2.596250285188431e-12</v>
       </c>
       <c r="D55" t="n">
-        <v>0.05464932477184229</v>
+        <v>0.9999964720821897</v>
       </c>
       <c r="E55" t="n">
-        <v>0.0008830306206513766</v>
+        <v>1.564955787799904e-09</v>
       </c>
       <c r="F55" t="n">
-        <v>0.9311485042443088</v>
+        <v>3.526350258260762e-06</v>
       </c>
     </row>
     <row r="56">
@@ -1733,20 +1733,20 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.9970876419481446</v>
+        <v>0.01471148749439908</v>
       </c>
       <c r="D56" t="n">
-        <v>7.017074963211012e-05</v>
+        <v>0.9852183171737979</v>
       </c>
       <c r="E56" t="n">
-        <v>0.0001335010119803655</v>
+        <v>2.445872329535962e-05</v>
       </c>
       <c r="F56" t="n">
-        <v>0.002708686290243477</v>
+        <v>4.573660850735519e-05</v>
       </c>
     </row>
     <row r="57">
@@ -1757,20 +1757,20 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.08126454008679292</v>
+        <v>1.529379669603779e-05</v>
       </c>
       <c r="D57" t="n">
-        <v>0.3479009519734195</v>
+        <v>0.9999585308610335</v>
       </c>
       <c r="E57" t="n">
-        <v>0.004147636301056327</v>
+        <v>2.147610908776933e-05</v>
       </c>
       <c r="F57" t="n">
-        <v>0.5666868716387313</v>
+        <v>4.6992331828087e-06</v>
       </c>
     </row>
     <row r="58">
@@ -1781,20 +1781,20 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.0009411322230673107</v>
+        <v>7.34642653984183e-05</v>
       </c>
       <c r="D58" t="n">
-        <v>0.009887117660395617</v>
+        <v>0.9985984977810332</v>
       </c>
       <c r="E58" t="n">
-        <v>0.9752196307049895</v>
+        <v>0.001327930800023401</v>
       </c>
       <c r="F58" t="n">
-        <v>0.01395211941154751</v>
+        <v>1.071535450503978e-07</v>
       </c>
     </row>
     <row r="59">
@@ -1805,20 +1805,20 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.0380987585695971</v>
+        <v>4.905701292933268e-05</v>
       </c>
       <c r="D59" t="n">
-        <v>0.01721955437805785</v>
+        <v>0.9998799879387282</v>
       </c>
       <c r="E59" t="n">
-        <v>0.8074667343925427</v>
+        <v>4.651479546930326e-07</v>
       </c>
       <c r="F59" t="n">
-        <v>0.1372149526598023</v>
+        <v>7.048990038772581e-05</v>
       </c>
     </row>
     <row r="60">
@@ -1829,20 +1829,20 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.1847767740949373</v>
+        <v>0.03932109614775176</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1306790823700288</v>
+        <v>0.04157183911787529</v>
       </c>
       <c r="E60" t="n">
-        <v>0.1563318774753384</v>
+        <v>0.9187946269492396</v>
       </c>
       <c r="F60" t="n">
-        <v>0.5282122660596955</v>
+        <v>0.000312437785133444</v>
       </c>
     </row>
     <row r="61">
@@ -1857,16 +1857,16 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.04982068825045143</v>
+        <v>1.521478377065248e-07</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2090051449685728</v>
+        <v>0.0008487884047503272</v>
       </c>
       <c r="E61" t="n">
-        <v>0.474815521680839</v>
+        <v>0.8686793250061724</v>
       </c>
       <c r="F61" t="n">
-        <v>0.2663586451001371</v>
+        <v>0.1304717344412396</v>
       </c>
     </row>
     <row r="62">
@@ -1881,16 +1881,16 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.01788202162282966</v>
+        <v>9.96662979616377e-07</v>
       </c>
       <c r="D62" t="n">
-        <v>0.08336170971836368</v>
+        <v>2.579429497580051e-10</v>
       </c>
       <c r="E62" t="n">
-        <v>0.4527089885261286</v>
+        <v>0.9991191505963533</v>
       </c>
       <c r="F62" t="n">
-        <v>0.446047280132678</v>
+        <v>0.0008798524827242317</v>
       </c>
     </row>
     <row r="63">
@@ -1901,20 +1901,20 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.002342730038518375</v>
+        <v>1.224689485325342e-10</v>
       </c>
       <c r="D63" t="n">
-        <v>0.01874987990457705</v>
+        <v>3.122574855577207e-06</v>
       </c>
       <c r="E63" t="n">
-        <v>0.3634789464963444</v>
+        <v>0.9999968703186549</v>
       </c>
       <c r="F63" t="n">
-        <v>0.6154284435605601</v>
+        <v>6.984020594648756e-09</v>
       </c>
     </row>
     <row r="64">
@@ -1925,20 +1925,20 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.01088158857862999</v>
+        <v>7.511285995843036e-07</v>
       </c>
       <c r="D64" t="n">
-        <v>0.03298322623575701</v>
+        <v>2.14167923579717e-05</v>
       </c>
       <c r="E64" t="n">
-        <v>0.1063184136629956</v>
+        <v>0.9914557952731075</v>
       </c>
       <c r="F64" t="n">
-        <v>0.8498167715226175</v>
+        <v>0.008522036805934897</v>
       </c>
     </row>
     <row r="65">
@@ -1953,16 +1953,16 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.01021158700357143</v>
+        <v>2.361910669225673e-07</v>
       </c>
       <c r="D65" t="n">
-        <v>0.00458337362136785</v>
+        <v>0.01233682166749172</v>
       </c>
       <c r="E65" t="n">
-        <v>0.6128418243999014</v>
+        <v>0.9677950419028893</v>
       </c>
       <c r="F65" t="n">
-        <v>0.3723632149751593</v>
+        <v>0.01986790023855198</v>
       </c>
     </row>
     <row r="66">
@@ -1973,20 +1973,20 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.03283825418528316</v>
+        <v>7.915476466624783e-08</v>
       </c>
       <c r="D66" t="n">
-        <v>0.01370644943371203</v>
+        <v>0.002238608604265795</v>
       </c>
       <c r="E66" t="n">
-        <v>0.4484489753463254</v>
+        <v>0.9977329899793137</v>
       </c>
       <c r="F66" t="n">
-        <v>0.5050063210346794</v>
+        <v>2.83222616556881e-05</v>
       </c>
     </row>
     <row r="67">
@@ -1997,20 +1997,20 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.02092377406254374</v>
+        <v>1.499169343524586e-08</v>
       </c>
       <c r="D67" t="n">
-        <v>0.01749718974694352</v>
+        <v>0.0002789672605150415</v>
       </c>
       <c r="E67" t="n">
-        <v>0.1628495858141605</v>
+        <v>0.9846742844342252</v>
       </c>
       <c r="F67" t="n">
-        <v>0.7987294503763522</v>
+        <v>0.01504673331356623</v>
       </c>
     </row>
     <row r="68">
@@ -2021,20 +2021,20 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.002350423950973783</v>
+        <v>0.003920491140580307</v>
       </c>
       <c r="D68" t="n">
-        <v>0.007240551165038419</v>
+        <v>0.003475230257418431</v>
       </c>
       <c r="E68" t="n">
-        <v>0.06217455800496971</v>
+        <v>0.788074558349959</v>
       </c>
       <c r="F68" t="n">
-        <v>0.9282344668790181</v>
+        <v>0.2045297202520422</v>
       </c>
     </row>
     <row r="69">
@@ -2045,20 +2045,20 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>incorrect angry</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.00243512581224943</v>
+        <v>0.9552573831052003</v>
       </c>
       <c r="D69" t="n">
-        <v>0.006175243307718647</v>
+        <v>0.01081140424899229</v>
       </c>
       <c r="E69" t="n">
-        <v>0.9415841381569668</v>
+        <v>0.0213036823350779</v>
       </c>
       <c r="F69" t="n">
-        <v>0.04980549272306525</v>
+        <v>0.01262753031072963</v>
       </c>
     </row>
     <row r="70">
@@ -2073,16 +2073,16 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.002168757091693651</v>
+        <v>0.0004724475864797445</v>
       </c>
       <c r="D70" t="n">
-        <v>0.009806424037568292</v>
+        <v>0.2341160154103321</v>
       </c>
       <c r="E70" t="n">
-        <v>0.4219450085658258</v>
+        <v>0.0005458522433986733</v>
       </c>
       <c r="F70" t="n">
-        <v>0.5660798103049124</v>
+        <v>0.7648656847597894</v>
       </c>
     </row>
     <row r="71">
@@ -2097,16 +2097,16 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.007934648959867898</v>
+        <v>3.143046021833847e-07</v>
       </c>
       <c r="D71" t="n">
-        <v>0.003976951620888842</v>
+        <v>1.834940797826558e-05</v>
       </c>
       <c r="E71" t="n">
-        <v>0.01544076505138055</v>
+        <v>9.127925978931998e-05</v>
       </c>
       <c r="F71" t="n">
-        <v>0.9726476343678627</v>
+        <v>0.9998900570276302</v>
       </c>
     </row>
     <row r="72">
@@ -2117,20 +2117,20 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>incorrect happy</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.1022201755587806</v>
+        <v>0.003251279096956241</v>
       </c>
       <c r="D72" t="n">
-        <v>0.3474953829640091</v>
+        <v>0.1378267693402731</v>
       </c>
       <c r="E72" t="n">
-        <v>0.2207682530560133</v>
+        <v>0.001521497588796765</v>
       </c>
       <c r="F72" t="n">
-        <v>0.3295161884211967</v>
+        <v>0.8574004539739739</v>
       </c>
     </row>
     <row r="73">
@@ -2145,16 +2145,16 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.002980680037855231</v>
+        <v>1.933607516250382e-10</v>
       </c>
       <c r="D73" t="n">
-        <v>0.01521446713556014</v>
+        <v>1.872457615146125e-07</v>
       </c>
       <c r="E73" t="n">
-        <v>0.1777813637693905</v>
+        <v>0.0001835744289245253</v>
       </c>
       <c r="F73" t="n">
-        <v>0.8040234890571942</v>
+        <v>0.9998162381319533</v>
       </c>
     </row>
     <row r="74">
@@ -2169,16 +2169,16 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.004492317114871837</v>
+        <v>2.026604843426401e-12</v>
       </c>
       <c r="D74" t="n">
-        <v>0.007266246629477249</v>
+        <v>0.0002849760237597858</v>
       </c>
       <c r="E74" t="n">
-        <v>0.3727510209706461</v>
+        <v>1.447478379325178e-05</v>
       </c>
       <c r="F74" t="n">
-        <v>0.6154904152850047</v>
+        <v>0.9997005491904204</v>
       </c>
     </row>
     <row r="75">
@@ -2193,16 +2193,16 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.002504843191026519</v>
+        <v>3.227199314638416e-15</v>
       </c>
       <c r="D75" t="n">
-        <v>0.007721362889234841</v>
+        <v>1.143436785918568e-06</v>
       </c>
       <c r="E75" t="n">
-        <v>0.04585785055999618</v>
+        <v>0.0002687122509892058</v>
       </c>
       <c r="F75" t="n">
-        <v>0.9439159433597424</v>
+        <v>0.9997301443122216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Combined predicting multiple and renamed files
</commit_message>
<xml_diff>
--- a/predict_from_audio/prediction.xlsx
+++ b/predict_from_audio/prediction.xlsx
@@ -459,6 +459,11 @@
           <t>emotion to predict</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>angry</t>
@@ -499,16 +504,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9999999980980918</v>
+        <v>0.9999999980980949</v>
       </c>
       <c r="D3" t="n">
-        <v>1.901908152575907e-09</v>
+        <v>1.901904995461747e-09</v>
       </c>
       <c r="E3" t="n">
-        <v>6.241178625482975e-28</v>
+        <v>6.241174249799297e-28</v>
       </c>
       <c r="F3" t="n">
-        <v>3.24068762193153e-26</v>
+        <v>3.240682417445794e-26</v>
       </c>
     </row>
     <row r="4">
@@ -523,16 +528,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9999999988419648</v>
+        <v>0.999999998841965</v>
       </c>
       <c r="D4" t="n">
-        <v>1.158035163895001e-09</v>
+        <v>1.158034996411025e-09</v>
       </c>
       <c r="E4" t="n">
-        <v>6.9807208838602e-32</v>
+        <v>6.980722501337461e-32</v>
       </c>
       <c r="F4" t="n">
-        <v>9.205529105521453e-28</v>
+        <v>9.205532364011098e-28</v>
       </c>
     </row>
     <row r="5">
@@ -547,16 +552,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.07978859772950675</v>
+        <v>0.07978859980044345</v>
       </c>
       <c r="D5" t="n">
-        <v>0.915950241603852</v>
+        <v>0.9159502409144837</v>
       </c>
       <c r="E5" t="n">
-        <v>4.03284255152515e-12</v>
+        <v>4.032831793283457e-12</v>
       </c>
       <c r="F5" t="n">
-        <v>0.004261160662608308</v>
+        <v>0.004261159281039986</v>
       </c>
     </row>
     <row r="6">
@@ -571,16 +576,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.7317215961819231</v>
+        <v>0.7317210975447825</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2682693124181322</v>
+        <v>0.2682698110611456</v>
       </c>
       <c r="E6" t="n">
-        <v>3.700705271353019e-13</v>
+        <v>3.700699728581861e-13</v>
       </c>
       <c r="F6" t="n">
-        <v>9.091399574511182e-06</v>
+        <v>9.091393701826096e-06</v>
       </c>
     </row>
     <row r="7">
@@ -595,16 +600,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9999998682229498</v>
+        <v>0.9999998682229603</v>
       </c>
       <c r="D7" t="n">
-        <v>1.317725146248232e-07</v>
+        <v>1.317725042460183e-07</v>
       </c>
       <c r="E7" t="n">
-        <v>3.596490645575583e-18</v>
+        <v>3.596487446349577e-18</v>
       </c>
       <c r="F7" t="n">
-        <v>4.535385146185481e-12</v>
+        <v>4.535386877627977e-12</v>
       </c>
     </row>
     <row r="8">
@@ -622,13 +627,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>7.247268564707396e-27</v>
+        <v>7.247266196792305e-27</v>
       </c>
       <c r="E8" t="n">
-        <v>1.825553619872027e-28</v>
+        <v>1.825553260132532e-28</v>
       </c>
       <c r="F8" t="n">
-        <v>1.443668456632889e-23</v>
+        <v>1.443668298779819e-23</v>
       </c>
     </row>
     <row r="9">
@@ -643,16 +648,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.076438624114156e-07</v>
+        <v>2.076439083439849e-07</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7552214762279843</v>
+        <v>0.7552216971032443</v>
       </c>
       <c r="E9" t="n">
-        <v>4.258497450727397e-15</v>
+        <v>4.25850075206077e-15</v>
       </c>
       <c r="F9" t="n">
-        <v>0.244778316128149</v>
+        <v>0.2447780952528432</v>
       </c>
     </row>
     <row r="10">
@@ -667,16 +672,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.359082569358502e-11</v>
+        <v>1.359080261351768e-11</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9974690308427606</v>
+        <v>0.9974690360061493</v>
       </c>
       <c r="E10" t="n">
-        <v>8.168723877804321e-17</v>
+        <v>8.168701301367645e-17</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00253096914364843</v>
+        <v>0.002530963980259865</v>
       </c>
     </row>
     <row r="11">
@@ -691,16 +696,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.341148972453739e-06</v>
+        <v>1.341144513429911e-06</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9999986427433988</v>
+        <v>0.9999986427478598</v>
       </c>
       <c r="E11" t="n">
-        <v>6.620795969253407e-14</v>
+        <v>6.620799574074445e-14</v>
       </c>
       <c r="F11" t="n">
-        <v>1.610756277991192e-08</v>
+        <v>1.610756060607794e-08</v>
       </c>
     </row>
     <row r="12">
@@ -715,16 +720,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8.159915161718975e-05</v>
+        <v>8.159914519369728e-05</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9998922519320573</v>
+        <v>0.9998922519225758</v>
       </c>
       <c r="E12" t="n">
-        <v>1.263083644464787e-18</v>
+        <v>1.263083087686047e-18</v>
       </c>
       <c r="F12" t="n">
-        <v>2.614891632553173e-05</v>
+        <v>2.614893223040751e-05</v>
       </c>
     </row>
     <row r="13">
@@ -739,16 +744,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3.611808599893745e-06</v>
+        <v>3.61181118423013e-06</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9999363203536533</v>
+        <v>0.9999363203517819</v>
       </c>
       <c r="E13" t="n">
-        <v>5.290326123811149e-15</v>
+        <v>5.290326597065848e-15</v>
       </c>
       <c r="F13" t="n">
-        <v>6.006783774129995e-05</v>
+        <v>6.006783702848341e-05</v>
       </c>
     </row>
     <row r="14">
@@ -763,16 +768,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1.136807163704048e-08</v>
+        <v>1.136806924038118e-08</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9999998836976471</v>
+        <v>0.99999988369745</v>
       </c>
       <c r="E14" t="n">
-        <v>1.049342790594607e-07</v>
+        <v>1.04934478614327e-07</v>
       </c>
       <c r="F14" t="n">
-        <v>2.213137904753125e-15</v>
+        <v>2.213139182359058e-15</v>
       </c>
     </row>
     <row r="15">
@@ -787,16 +792,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1.788905429021265e-06</v>
+        <v>1.788907338548295e-06</v>
       </c>
       <c r="D15" t="n">
-        <v>2.324239124415401e-07</v>
+        <v>2.324238200162452e-07</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9989152990127276</v>
+        <v>0.9989152986799213</v>
       </c>
       <c r="F15" t="n">
-        <v>0.001082679657930955</v>
+        <v>0.001082679988919947</v>
       </c>
     </row>
     <row r="16">
@@ -811,16 +816,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4.825020100563713e-13</v>
+        <v>4.825025453316284e-13</v>
       </c>
       <c r="D16" t="n">
-        <v>4.755995081681969e-06</v>
+        <v>4.755995859410626e-06</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9999925942116565</v>
+        <v>0.9999925942100356</v>
       </c>
       <c r="F16" t="n">
-        <v>2.649792779297926e-06</v>
+        <v>2.649793622348031e-06</v>
       </c>
     </row>
     <row r="17">
@@ -835,16 +840,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.267385917871837e-14</v>
+        <v>5.267398557122042e-14</v>
       </c>
       <c r="D17" t="n">
-        <v>5.91386014091039e-14</v>
+        <v>5.913860667544247e-14</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9999999997338691</v>
+        <v>0.9999999997338693</v>
       </c>
       <c r="F17" t="n">
-        <v>2.660188942789926e-10</v>
+        <v>2.660187922800145e-10</v>
       </c>
     </row>
     <row r="18">
@@ -859,16 +864,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>9.167849298109255e-07</v>
+        <v>9.167844830720351e-07</v>
       </c>
       <c r="D18" t="n">
-        <v>1.380257509500387e-12</v>
+        <v>1.38025772107996e-12</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2170218620673969</v>
+        <v>0.217021513800701</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7829772211462931</v>
+        <v>0.7829775694134358</v>
       </c>
     </row>
     <row r="19">
@@ -883,16 +888,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.002521283185271597</v>
+        <v>0.002521291358893198</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0003114556458699814</v>
+        <v>0.0003114562656439268</v>
       </c>
       <c r="E19" t="n">
-        <v>1.201146502889526e-05</v>
+        <v>1.201148901863175e-05</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9971552497038294</v>
+        <v>0.9971552408864441</v>
       </c>
     </row>
     <row r="20">
@@ -907,16 +912,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.627230495322843e-28</v>
+        <v>1.627233266034137e-28</v>
       </c>
       <c r="D20" t="n">
-        <v>1.108152862671469e-15</v>
+        <v>1.108153774846515e-15</v>
       </c>
       <c r="E20" t="n">
         <v>0.9999999999999989</v>
       </c>
       <c r="F20" t="n">
-        <v>4.847583700422469e-24</v>
+        <v>4.8475913277978e-24</v>
       </c>
     </row>
     <row r="21">
@@ -931,16 +936,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>9.872802888308033e-05</v>
+        <v>9.872791293575983e-05</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9996306605983805</v>
+        <v>0.9996306604091083</v>
       </c>
       <c r="E21" t="n">
-        <v>1.88507559351379e-07</v>
+        <v>1.885074527408338e-07</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0002704228651769976</v>
+        <v>0.0002704231705033169</v>
       </c>
     </row>
     <row r="22">
@@ -955,13 +960,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.043999183178242e-13</v>
+        <v>1.043999271586192e-13</v>
       </c>
       <c r="D22" t="n">
-        <v>2.563088372874556e-08</v>
+        <v>2.563088381796272e-08</v>
       </c>
       <c r="E22" t="n">
-        <v>1.419079391266617e-17</v>
+        <v>1.419079235146876e-17</v>
       </c>
       <c r="F22" t="n">
         <v>0.9999999743690118</v>
@@ -979,16 +984,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>7.864140492484909e-08</v>
+        <v>7.864135314491153e-08</v>
       </c>
       <c r="D23" t="n">
-        <v>1.207828392708157e-05</v>
+        <v>1.207827015908761e-05</v>
       </c>
       <c r="E23" t="n">
-        <v>8.623856834011515e-10</v>
+        <v>8.623843746223741e-10</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9999878422122824</v>
+        <v>0.9999878422261035</v>
       </c>
     </row>
     <row r="24">
@@ -1003,16 +1008,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9.441774953955721e-05</v>
+        <v>9.441797537633337e-05</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0009011389545672526</v>
+        <v>0.0009011411857433194</v>
       </c>
       <c r="E24" t="n">
-        <v>1.801610623829556e-06</v>
+        <v>1.801617216929928e-06</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9990026416852694</v>
+        <v>0.9990026392216633</v>
       </c>
     </row>
     <row r="25">
@@ -1027,16 +1032,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.0005691952652516235</v>
+        <v>0.0005691957211546235</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01157272178444115</v>
+        <v>0.01157271473250004</v>
       </c>
       <c r="E25" t="n">
-        <v>2.11764463441168e-09</v>
+        <v>2.117646833810993e-09</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9878580808326626</v>
+        <v>0.9878580874286984</v>
       </c>
     </row>
     <row r="26">
@@ -1051,16 +1056,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.000429987230323094</v>
+        <v>0.0004299863567192703</v>
       </c>
       <c r="D26" t="n">
-        <v>6.171799975852523e-05</v>
+        <v>6.17178834904341e-05</v>
       </c>
       <c r="E26" t="n">
-        <v>3.53057221793778e-16</v>
+        <v>3.530565868931348e-16</v>
       </c>
       <c r="F26" t="n">
-        <v>0.999508294769918</v>
+        <v>0.9995082957597899</v>
       </c>
     </row>
     <row r="27">
@@ -1075,16 +1080,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.0005401609236637914</v>
+        <v>0.0005401626535553298</v>
       </c>
       <c r="D27" t="n">
-        <v>0.000198378222293387</v>
+        <v>0.0001983783113148826</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9991767897316592</v>
+        <v>0.9991767881512397</v>
       </c>
       <c r="F27" t="n">
-        <v>8.467112238363382e-05</v>
+        <v>8.467088389010569e-05</v>
       </c>
     </row>
     <row r="28">
@@ -1106,16 +1111,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.0814425560285887</v>
+        <v>0.08144257809034104</v>
       </c>
       <c r="D29" t="n">
-        <v>0.9185573502682775</v>
+        <v>0.9185573282066218</v>
       </c>
       <c r="E29" t="n">
-        <v>9.370313391330304e-08</v>
+        <v>9.370303720305335e-08</v>
       </c>
       <c r="F29" t="n">
-        <v>5.309634488989088e-22</v>
+        <v>5.309629061437822e-22</v>
       </c>
     </row>
     <row r="30">
@@ -1130,16 +1135,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.9985732142207621</v>
+        <v>0.998573212519375</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0003990740848488969</v>
+        <v>0.0003990742876771093</v>
       </c>
       <c r="E30" t="n">
-        <v>0.001025864727617267</v>
+        <v>0.001025866223749394</v>
       </c>
       <c r="F30" t="n">
-        <v>1.846966771687364e-06</v>
+        <v>1.846969198455936e-06</v>
       </c>
     </row>
     <row r="31">
@@ -1154,16 +1159,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.01288722464345116</v>
+        <v>0.01288723940169992</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0002606971997256433</v>
+        <v>0.0002606973730451644</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9868520781567823</v>
+        <v>0.9868520632252141</v>
       </c>
       <c r="F31" t="n">
-        <v>4.065066838881868e-14</v>
+        <v>4.06506964265733e-14</v>
       </c>
     </row>
     <row r="32">
@@ -1178,16 +1183,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1.426009818619849e-09</v>
+        <v>1.426009519948071e-09</v>
       </c>
       <c r="D32" t="n">
-        <v>0.8896752896596947</v>
+        <v>0.8896752737063891</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0001206871018144671</v>
+        <v>0.0001206871310782763</v>
       </c>
       <c r="F32" t="n">
-        <v>0.1102040218124811</v>
+        <v>0.110204037736523</v>
       </c>
     </row>
     <row r="33">
@@ -1202,16 +1207,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3.503649579178466e-05</v>
+        <v>3.503645296559549e-05</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0347793659543468</v>
+        <v>0.03477933168817512</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9651773564297866</v>
+        <v>0.9651773907415127</v>
       </c>
       <c r="F33" t="n">
-        <v>8.241120074756249e-06</v>
+        <v>8.241117346439033e-06</v>
       </c>
     </row>
     <row r="34">
@@ -1226,16 +1231,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4.014697095164784e-05</v>
+        <v>4.014689492725665e-05</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9986293315232968</v>
+        <v>0.9986293339753848</v>
       </c>
       <c r="E34" t="n">
-        <v>0.001330520708528741</v>
+        <v>0.001330518332464757</v>
       </c>
       <c r="F34" t="n">
-        <v>7.972228314141262e-10</v>
+        <v>7.972231476719833e-10</v>
       </c>
     </row>
     <row r="35">
@@ -1250,16 +1255,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1.943800064090439e-08</v>
+        <v>1.943800643359612e-08</v>
       </c>
       <c r="D35" t="n">
-        <v>4.086935124253035e-07</v>
+        <v>4.086933765320614e-07</v>
       </c>
       <c r="E35" t="n">
-        <v>0.9999995714443086</v>
+        <v>0.9999995714444387</v>
       </c>
       <c r="F35" t="n">
-        <v>4.241783356967995e-10</v>
+        <v>4.241782555792451e-10</v>
       </c>
     </row>
     <row r="36">
@@ -1274,16 +1279,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1.403596674930701e-09</v>
+        <v>1.403598953564861e-09</v>
       </c>
       <c r="D36" t="n">
-        <v>1.185880567598732e-06</v>
+        <v>1.185882010835925e-06</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9999873566523821</v>
+        <v>0.999987356642669</v>
       </c>
       <c r="F36" t="n">
-        <v>1.145606345365589e-05</v>
+        <v>1.145607172124487e-05</v>
       </c>
     </row>
     <row r="37">
@@ -1298,16 +1303,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1.226635068154167e-11</v>
+        <v>1.226635163855063e-11</v>
       </c>
       <c r="D37" t="n">
-        <v>4.884522802381617e-09</v>
+        <v>4.884523151363319e-09</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9999999942280866</v>
+        <v>0.9999999942280855</v>
       </c>
       <c r="F37" t="n">
-        <v>8.751242892619664e-10</v>
+        <v>8.751248385225806e-10</v>
       </c>
     </row>
     <row r="38">
@@ -1322,16 +1327,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4.306242226912951e-10</v>
+        <v>4.30622990737897e-10</v>
       </c>
       <c r="D38" t="n">
-        <v>1.777426296487112e-09</v>
+        <v>1.777424020284196e-09</v>
       </c>
       <c r="E38" t="n">
-        <v>0.9999999961169554</v>
+        <v>0.9999999961169608</v>
       </c>
       <c r="F38" t="n">
-        <v>1.674993918355791e-09</v>
+        <v>1.674992057146099e-09</v>
       </c>
     </row>
     <row r="39">
@@ -1346,16 +1351,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1.208491988796428e-12</v>
+        <v>1.208492254400782e-12</v>
       </c>
       <c r="D39" t="n">
-        <v>9.4144957652019e-11</v>
+        <v>9.414490715148804e-11</v>
       </c>
       <c r="E39" t="n">
         <v>0.9999999998804396</v>
       </c>
       <c r="F39" t="n">
-        <v>2.420687821437202e-11</v>
+        <v>2.420688105771143e-11</v>
       </c>
     </row>
     <row r="40">
@@ -1370,16 +1375,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>6.734878510948267e-14</v>
+        <v>6.734879062730671e-14</v>
       </c>
       <c r="D40" t="n">
-        <v>9.296465752113463e-10</v>
+        <v>9.296461668540372e-10</v>
       </c>
       <c r="E40" t="n">
-        <v>0.9999999990700406</v>
+        <v>0.999999999070041</v>
       </c>
       <c r="F40" t="n">
-        <v>2.454941920588478e-13</v>
+        <v>2.454941885365347e-13</v>
       </c>
     </row>
     <row r="41">
@@ -1394,16 +1399,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.291918655052882e-09</v>
+        <v>1.291918045288698e-09</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0008702119792345535</v>
+        <v>0.0008702118631205627</v>
       </c>
       <c r="E41" t="n">
-        <v>0.9962375563123423</v>
+        <v>0.9962375562299454</v>
       </c>
       <c r="F41" t="n">
-        <v>0.002892230416504446</v>
+        <v>0.002892230615016065</v>
       </c>
     </row>
     <row r="42">
@@ -1418,16 +1423,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1.776056614694799e-14</v>
+        <v>1.776057772770287e-14</v>
       </c>
       <c r="D42" t="n">
-        <v>8.252562008742703e-12</v>
+        <v>8.25256065935441e-12</v>
       </c>
       <c r="E42" t="n">
-        <v>0.009795382846568869</v>
+        <v>0.009795388217495248</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9902046171451608</v>
+        <v>0.9902046117742345</v>
       </c>
     </row>
     <row r="43">
@@ -1449,16 +1454,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.03130013732308146</v>
+        <v>0.03130012115633713</v>
       </c>
       <c r="D44" t="n">
-        <v>0.9686998321688762</v>
+        <v>0.9686998483356055</v>
       </c>
       <c r="E44" t="n">
-        <v>2.73405502151761e-08</v>
+        <v>2.734056260570158e-08</v>
       </c>
       <c r="F44" t="n">
-        <v>3.167491882656891e-09</v>
+        <v>3.167494693366019e-09</v>
       </c>
     </row>
     <row r="45">
@@ -1473,16 +1478,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.9999997658712945</v>
+        <v>0.9999997658713984</v>
       </c>
       <c r="D45" t="n">
-        <v>2.341253064950237e-07</v>
+        <v>2.341252026837822e-07</v>
       </c>
       <c r="E45" t="n">
-        <v>3.393911730012946e-12</v>
+        <v>3.393910339747311e-12</v>
       </c>
       <c r="F45" t="n">
-        <v>5.170900987975009e-15</v>
+        <v>5.170899353180098e-15</v>
       </c>
     </row>
     <row r="46">
@@ -1497,16 +1502,16 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.9999999827512297</v>
+        <v>0.9999999827512501</v>
       </c>
       <c r="D46" t="n">
-        <v>1.724808539883253e-08</v>
+        <v>1.724806482086797e-08</v>
       </c>
       <c r="E46" t="n">
-        <v>9.051866816753053e-16</v>
+        <v>9.051858930645069e-16</v>
       </c>
       <c r="F46" t="n">
-        <v>6.841270024694351e-13</v>
+        <v>6.841267732129574e-13</v>
       </c>
     </row>
     <row r="47">
@@ -1521,16 +1526,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.9999981489460259</v>
+        <v>0.9999981489438758</v>
       </c>
       <c r="D47" t="n">
-        <v>1.805580582609897e-06</v>
+        <v>1.80558268397725e-06</v>
       </c>
       <c r="E47" t="n">
-        <v>4.525431365029557e-08</v>
+        <v>4.525436208148148e-08</v>
       </c>
       <c r="F47" t="n">
-        <v>2.190778614993478e-10</v>
+        <v>2.19078121362754e-10</v>
       </c>
     </row>
     <row r="48">
@@ -1545,16 +1550,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.3618318166648764</v>
+        <v>0.3618317492240281</v>
       </c>
       <c r="D48" t="n">
-        <v>0.6381647473595103</v>
+        <v>0.6381648147985317</v>
       </c>
       <c r="E48" t="n">
-        <v>2.887581689093385e-08</v>
+        <v>2.887581080372506e-08</v>
       </c>
       <c r="F48" t="n">
-        <v>3.407099796163236e-06</v>
+        <v>3.407101629380745e-06</v>
       </c>
     </row>
     <row r="49">
@@ -1569,16 +1574,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.6473000818358808</v>
+        <v>0.6473000232512405</v>
       </c>
       <c r="D49" t="n">
-        <v>0.3526649760793807</v>
+        <v>0.3526650346501983</v>
       </c>
       <c r="E49" t="n">
-        <v>3.421235727185909e-05</v>
+        <v>3.421237152200893e-05</v>
       </c>
       <c r="F49" t="n">
-        <v>7.297274665193926e-07</v>
+        <v>7.297270392678669e-07</v>
       </c>
     </row>
     <row r="50">
@@ -1593,16 +1598,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.9999999910402405</v>
+        <v>0.9999999910402356</v>
       </c>
       <c r="D50" t="n">
-        <v>8.959626294145054e-09</v>
+        <v>8.959631283248769e-09</v>
       </c>
       <c r="E50" t="n">
-        <v>1.333085419509235e-13</v>
+        <v>1.333084195262829e-13</v>
       </c>
       <c r="F50" t="n">
-        <v>1.985225483841853e-18</v>
+        <v>1.985223505090241e-18</v>
       </c>
     </row>
     <row r="51">
@@ -1617,16 +1622,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.9999999988311012</v>
+        <v>0.999999998831099</v>
       </c>
       <c r="D51" t="n">
-        <v>1.031173686272702e-09</v>
+        <v>1.031175101648718e-09</v>
       </c>
       <c r="E51" t="n">
-        <v>1.113750939167807e-10</v>
+        <v>1.113755147489007e-10</v>
       </c>
       <c r="F51" t="n">
-        <v>2.635010776557755e-11</v>
+        <v>2.635023075646463e-11</v>
       </c>
     </row>
     <row r="52">
@@ -1641,16 +1646,16 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.02352517099769824</v>
+        <v>0.02352518849867759</v>
       </c>
       <c r="D52" t="n">
-        <v>0.8052797136071453</v>
+        <v>0.8052797140541254</v>
       </c>
       <c r="E52" t="n">
-        <v>0.1711946884165533</v>
+        <v>0.1711946704690515</v>
       </c>
       <c r="F52" t="n">
-        <v>4.269786029598599e-07</v>
+        <v>4.269781455912076e-07</v>
       </c>
     </row>
     <row r="53">
@@ -1665,16 +1670,16 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.0003463828112435817</v>
+        <v>0.0003463831908508977</v>
       </c>
       <c r="D53" t="n">
-        <v>0.9992461016441622</v>
+        <v>0.9992461014184022</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0003926137395219223</v>
+        <v>0.0003926135806871011</v>
       </c>
       <c r="F53" t="n">
-        <v>1.490180507246497e-05</v>
+        <v>1.490181005985252e-05</v>
       </c>
     </row>
     <row r="54">
@@ -1689,16 +1694,16 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2.123060364492161e-07</v>
+        <v>2.123056368302282e-07</v>
       </c>
       <c r="D54" t="n">
-        <v>0.9999997812632376</v>
+        <v>0.9999997812636404</v>
       </c>
       <c r="E54" t="n">
-        <v>6.405090017418388e-09</v>
+        <v>6.405086820697973e-09</v>
       </c>
       <c r="F54" t="n">
-        <v>2.563597522620052e-11</v>
+        <v>2.56359605192664e-11</v>
       </c>
     </row>
     <row r="55">
@@ -1713,16 +1718,16 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2.596250285188431e-12</v>
+        <v>2.59625020154014e-12</v>
       </c>
       <c r="D55" t="n">
-        <v>0.9999964720821897</v>
+        <v>0.9999964720816381</v>
       </c>
       <c r="E55" t="n">
-        <v>1.564955787799904e-09</v>
+        <v>1.564956279207119e-09</v>
       </c>
       <c r="F55" t="n">
-        <v>3.526350258260762e-06</v>
+        <v>3.526350809429424e-06</v>
       </c>
     </row>
     <row r="56">
@@ -1737,16 +1742,16 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.01471148749439908</v>
+        <v>0.01471149268719845</v>
       </c>
       <c r="D56" t="n">
-        <v>0.9852183171737979</v>
+        <v>0.9852183119320149</v>
       </c>
       <c r="E56" t="n">
-        <v>2.445872329535962e-05</v>
+        <v>2.445873555954392e-05</v>
       </c>
       <c r="F56" t="n">
-        <v>4.573660850735519e-05</v>
+        <v>4.573664522715527e-05</v>
       </c>
     </row>
     <row r="57">
@@ -1761,16 +1766,16 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1.529379669603779e-05</v>
+        <v>1.529380350351737e-05</v>
       </c>
       <c r="D57" t="n">
-        <v>0.9999585308610335</v>
+        <v>0.9999585308344019</v>
       </c>
       <c r="E57" t="n">
-        <v>2.147610908776933e-05</v>
+        <v>2.147612830633627e-05</v>
       </c>
       <c r="F57" t="n">
-        <v>4.6992331828087e-06</v>
+        <v>4.699233788076977e-06</v>
       </c>
     </row>
     <row r="58">
@@ -1785,16 +1790,16 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>7.34642653984183e-05</v>
+        <v>7.346427186821857e-05</v>
       </c>
       <c r="D58" t="n">
-        <v>0.9985984977810332</v>
+        <v>0.9985984970367721</v>
       </c>
       <c r="E58" t="n">
-        <v>0.001327930800023401</v>
+        <v>0.001327931537802398</v>
       </c>
       <c r="F58" t="n">
-        <v>1.071535450503978e-07</v>
+        <v>1.071535573377898e-07</v>
       </c>
     </row>
     <row r="59">
@@ -1809,16 +1814,16 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>4.905701292933268e-05</v>
+        <v>4.905694321162588e-05</v>
       </c>
       <c r="D59" t="n">
-        <v>0.9998799879387282</v>
+        <v>0.999879988054084</v>
       </c>
       <c r="E59" t="n">
-        <v>4.651479546930326e-07</v>
+        <v>4.651476801232238e-07</v>
       </c>
       <c r="F59" t="n">
-        <v>7.048990038772581e-05</v>
+        <v>7.048985502420139e-05</v>
       </c>
     </row>
     <row r="60">
@@ -1833,16 +1838,16 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.03932109614775176</v>
+        <v>0.03932102878316885</v>
       </c>
       <c r="D60" t="n">
-        <v>0.04157183911787529</v>
+        <v>0.04157180779323957</v>
       </c>
       <c r="E60" t="n">
-        <v>0.9187946269492396</v>
+        <v>0.91879472569947</v>
       </c>
       <c r="F60" t="n">
-        <v>0.000312437785133444</v>
+        <v>0.0003124377241216265</v>
       </c>
     </row>
     <row r="61">
@@ -1857,16 +1862,16 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1.521478377065248e-07</v>
+        <v>1.521476539800239e-07</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0008487884047503272</v>
+        <v>0.0008487881057721555</v>
       </c>
       <c r="E61" t="n">
-        <v>0.8686793250061724</v>
+        <v>0.8686793674612773</v>
       </c>
       <c r="F61" t="n">
-        <v>0.1304717344412396</v>
+        <v>0.1304716922852966</v>
       </c>
     </row>
     <row r="62">
@@ -1881,16 +1886,16 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>9.96662979616377e-07</v>
+        <v>9.966631207651111e-07</v>
       </c>
       <c r="D62" t="n">
-        <v>2.579429497580051e-10</v>
+        <v>2.57942715782938e-10</v>
       </c>
       <c r="E62" t="n">
-        <v>0.9991191505963533</v>
+        <v>0.9991191509556385</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0008798524827242317</v>
+        <v>0.0008798521232979835</v>
       </c>
     </row>
     <row r="63">
@@ -1905,16 +1910,16 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1.224689485325342e-10</v>
+        <v>1.224690534897892e-10</v>
       </c>
       <c r="D63" t="n">
-        <v>3.122574855577207e-06</v>
+        <v>3.122577511005219e-06</v>
       </c>
       <c r="E63" t="n">
-        <v>0.9999968703186549</v>
+        <v>0.9999968703159957</v>
       </c>
       <c r="F63" t="n">
-        <v>6.984020594648756e-09</v>
+        <v>6.984024218849883e-09</v>
       </c>
     </row>
     <row r="64">
@@ -1929,16 +1934,16 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>7.511285995843036e-07</v>
+        <v>7.511285807726668e-07</v>
       </c>
       <c r="D64" t="n">
-        <v>2.14167923579717e-05</v>
+        <v>2.141678864751088e-05</v>
       </c>
       <c r="E64" t="n">
-        <v>0.9914557952731075</v>
+        <v>0.9914557949143274</v>
       </c>
       <c r="F64" t="n">
-        <v>0.008522036805934897</v>
+        <v>0.008522037168444452</v>
       </c>
     </row>
     <row r="65">
@@ -1953,16 +1958,16 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2.361910669225673e-07</v>
+        <v>2.361907307238748e-07</v>
       </c>
       <c r="D65" t="n">
-        <v>0.01233682166749172</v>
+        <v>0.01233680889919175</v>
       </c>
       <c r="E65" t="n">
-        <v>0.9677950419028893</v>
+        <v>0.9677950749510463</v>
       </c>
       <c r="F65" t="n">
-        <v>0.01986790023855198</v>
+        <v>0.01986787995903112</v>
       </c>
     </row>
     <row r="66">
@@ -1977,16 +1982,16 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>7.915476466624783e-08</v>
+        <v>7.915490148003956e-08</v>
       </c>
       <c r="D66" t="n">
-        <v>0.002238608604265795</v>
+        <v>0.002238612454534579</v>
       </c>
       <c r="E66" t="n">
-        <v>0.9977329899793137</v>
+        <v>0.997732986094622</v>
       </c>
       <c r="F66" t="n">
-        <v>2.83222616556881e-05</v>
+        <v>2.832229594211349e-05</v>
       </c>
     </row>
     <row r="67">
@@ -2001,16 +2006,16 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.499169343524586e-08</v>
+        <v>1.49917375319637e-08</v>
       </c>
       <c r="D67" t="n">
-        <v>0.0002789672605150415</v>
+        <v>0.000278967735139921</v>
       </c>
       <c r="E67" t="n">
-        <v>0.9846742844342252</v>
+        <v>0.984674273297942</v>
       </c>
       <c r="F67" t="n">
-        <v>0.01504673331356623</v>
+        <v>0.01504674397518064</v>
       </c>
     </row>
     <row r="68">
@@ -2025,16 +2030,16 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.003920491140580307</v>
+        <v>0.003920491024751745</v>
       </c>
       <c r="D68" t="n">
-        <v>0.003475230257418431</v>
+        <v>0.00347523334142926</v>
       </c>
       <c r="E68" t="n">
-        <v>0.788074558349959</v>
+        <v>0.7880747211989104</v>
       </c>
       <c r="F68" t="n">
-        <v>0.2045297202520422</v>
+        <v>0.2045295544349086</v>
       </c>
     </row>
     <row r="69">
@@ -2049,16 +2054,16 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.9552573831052003</v>
+        <v>0.9552573600481038</v>
       </c>
       <c r="D69" t="n">
-        <v>0.01081140424899229</v>
+        <v>0.01081141247446618</v>
       </c>
       <c r="E69" t="n">
-        <v>0.0213036823350779</v>
+        <v>0.02130369864989802</v>
       </c>
       <c r="F69" t="n">
-        <v>0.01262753031072963</v>
+        <v>0.01262752882753212</v>
       </c>
     </row>
     <row r="70">
@@ -2073,16 +2078,16 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.0004724475864797445</v>
+        <v>0.0004724475040417419</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2341160154103321</v>
+        <v>0.2341160541966946</v>
       </c>
       <c r="E70" t="n">
-        <v>0.0005458522433986733</v>
+        <v>0.0005458520238284552</v>
       </c>
       <c r="F70" t="n">
-        <v>0.7648656847597894</v>
+        <v>0.7648656462754353</v>
       </c>
     </row>
     <row r="71">
@@ -2097,16 +2102,16 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>3.143046021833847e-07</v>
+        <v>3.143042894919002e-07</v>
       </c>
       <c r="D71" t="n">
-        <v>1.834940797826558e-05</v>
+        <v>1.834940301789438e-05</v>
       </c>
       <c r="E71" t="n">
-        <v>9.127925978931998e-05</v>
+        <v>9.127923542763181e-05</v>
       </c>
       <c r="F71" t="n">
-        <v>0.9998900570276302</v>
+        <v>0.9998900570572651</v>
       </c>
     </row>
     <row r="72">
@@ -2121,16 +2126,16 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.003251279096956241</v>
+        <v>0.003251279397865645</v>
       </c>
       <c r="D72" t="n">
-        <v>0.1378267693402731</v>
+        <v>0.1378267186833491</v>
       </c>
       <c r="E72" t="n">
-        <v>0.001521497588796765</v>
+        <v>0.001521496953566769</v>
       </c>
       <c r="F72" t="n">
-        <v>0.8574004539739739</v>
+        <v>0.8574005049652186</v>
       </c>
     </row>
     <row r="73">
@@ -2145,16 +2150,16 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1.933607516250382e-10</v>
+        <v>1.933608171592541e-10</v>
       </c>
       <c r="D73" t="n">
-        <v>1.872457615146125e-07</v>
+        <v>1.872458002424772e-07</v>
       </c>
       <c r="E73" t="n">
-        <v>0.0001835744289245253</v>
+        <v>0.0001835745500298561</v>
       </c>
       <c r="F73" t="n">
-        <v>0.9998162381319533</v>
+        <v>0.999816238010809</v>
       </c>
     </row>
     <row r="74">
@@ -2169,16 +2174,16 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2.026604843426401e-12</v>
+        <v>2.026604839931455e-12</v>
       </c>
       <c r="D74" t="n">
-        <v>0.0002849760237597858</v>
+        <v>0.0002849758667794369</v>
       </c>
       <c r="E74" t="n">
-        <v>1.447478379325178e-05</v>
+        <v>1.447478911737849e-05</v>
       </c>
       <c r="F74" t="n">
-        <v>0.9997005491904204</v>
+        <v>0.9997005493420765</v>
       </c>
     </row>
     <row r="75">
@@ -2193,16 +2198,16 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>3.227199314638416e-15</v>
+        <v>3.227199690806363e-15</v>
       </c>
       <c r="D75" t="n">
-        <v>1.143436785918568e-06</v>
+        <v>1.143435977244247e-06</v>
       </c>
       <c r="E75" t="n">
-        <v>0.0002687122509892058</v>
+        <v>0.0002687121545531161</v>
       </c>
       <c r="F75" t="n">
-        <v>0.9997301443122216</v>
+        <v>0.9997301444094664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added intensity and created functions to predict multiple
</commit_message>
<xml_diff>
--- a/predict_from_audio/prediction.xlsx
+++ b/predict_from_audio/prediction.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,30 +456,35 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>emotion to predict</t>
+          <t>True emotion</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>result</t>
+          <t>Intensity</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>angry</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>happy</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>neutral</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>sad</t>
         </is>
@@ -500,19 +505,24 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>0.9999999980980949</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>1.901904995461747e-09</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>6.241174249799297e-28</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>3.240682417445794e-26</v>
       </c>
     </row>
@@ -524,19 +534,24 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>0.999999998841965</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>1.158034996411025e-09</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>6.980722501337461e-32</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>9.205532364011098e-28</v>
       </c>
     </row>
@@ -548,19 +563,24 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>incorrect happy</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0.07978859980044345</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>0.9159502409144837</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>4.032831793283457e-12</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>0.004261159281039986</v>
       </c>
     </row>
@@ -572,19 +592,24 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>0.7317210975447825</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>0.2682698110611456</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>3.700699728581861e-13</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>9.091393701826096e-06</v>
       </c>
     </row>
@@ -596,19 +621,24 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>0.9999998682229603</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>1.317725042460183e-07</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>3.596487446349577e-18</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>4.535386877627977e-12</v>
       </c>
     </row>
@@ -620,19 +650,24 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>1</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>7.247266196792305e-27</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>1.825553260132532e-28</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>1.443668298779819e-23</v>
       </c>
     </row>
@@ -644,19 +679,24 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>2.076439083439849e-07</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>0.7552216971032443</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>4.25850075206077e-15</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>0.2447780952528432</v>
       </c>
     </row>
@@ -668,19 +708,24 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>1.359080261351768e-11</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>0.9974690360061493</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>8.168701301367645e-17</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>0.002530963980259865</v>
       </c>
     </row>
@@ -692,19 +737,24 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>1.341144513429911e-06</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>0.9999986427478598</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>6.620799574074445e-14</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>1.610756060607794e-08</v>
       </c>
     </row>
@@ -716,19 +766,24 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>8.159914519369728e-05</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>0.9998922519225758</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>1.263083087686047e-18</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>2.614893223040751e-05</v>
       </c>
     </row>
@@ -740,19 +795,24 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>3.61181118423013e-06</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>0.9999363203517819</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>5.290326597065848e-15</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>6.006783702848341e-05</v>
       </c>
     </row>
@@ -764,19 +824,24 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>1.136806924038118e-08</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>0.99999988369745</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>1.04934478614327e-07</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>2.213139182359058e-15</v>
       </c>
     </row>
@@ -788,19 +853,24 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
         <v>1.788907338548295e-06</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>2.324238200162452e-07</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>0.9989152986799213</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>0.001082679988919947</v>
       </c>
     </row>
@@ -812,19 +882,24 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>4.825025453316284e-13</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>4.755995859410626e-06</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>0.9999925942100356</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>2.649793622348031e-06</v>
       </c>
     </row>
@@ -836,19 +911,24 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
         <v>5.267398557122042e-14</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>5.913860667544247e-14</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>0.9999999997338693</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>2.660187922800145e-10</v>
       </c>
     </row>
@@ -860,19 +940,24 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>incorrect sad</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>9.167844830720351e-07</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>1.38025772107996e-12</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>0.217021513800701</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>0.7829775694134358</v>
       </c>
     </row>
@@ -884,19 +969,24 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>incorrect sad</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>0.002521291358893198</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>0.0003114562656439268</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>1.201148901863175e-05</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>0.9971552408864441</v>
       </c>
     </row>
@@ -908,19 +998,24 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
         <v>1.627233266034137e-28</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>1.108153774846515e-15</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>0.9999999999999989</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>4.8475913277978e-24</v>
       </c>
     </row>
@@ -932,19 +1027,24 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>incorrect happy</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>9.872791293575983e-05</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>0.9996306604091083</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>1.885074527408338e-07</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>0.0002704231705033169</v>
       </c>
     </row>
@@ -956,19 +1056,24 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
         <v>1.043999271586192e-13</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>2.563088381796272e-08</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>1.419079235146876e-17</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>0.9999999743690118</v>
       </c>
     </row>
@@ -980,19 +1085,24 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
         <v>7.864135314491153e-08</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>1.207827015908761e-05</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>8.623843746223741e-10</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>0.9999878422261035</v>
       </c>
     </row>
@@ -1004,19 +1114,24 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
         <v>9.441797537633337e-05</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>0.0009011411857433194</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>1.801617216929928e-06</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>0.9990026392216633</v>
       </c>
     </row>
@@ -1028,19 +1143,24 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
         <v>0.0005691957211546235</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>0.01157271473250004</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>2.117646833810993e-09</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>0.9878580874286984</v>
       </c>
     </row>
@@ -1052,19 +1172,24 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
         <v>0.0004299863567192703</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>6.17178834904341e-05</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>3.530565868931348e-16</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>0.9995082957597899</v>
       </c>
     </row>
@@ -1076,19 +1201,24 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>incorrect neutral</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>0.0005401626535553298</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>0.0001983783113148826</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>0.9991767881512397</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>8.467088389010569e-05</v>
       </c>
     </row>
@@ -1107,20 +1237,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>incorrect happy</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>0.08144257809034104</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D29" t="n">
-        <v>0.9185573282066218</v>
+        <v>0.998573212519375</v>
       </c>
       <c r="E29" t="n">
-        <v>9.370303720305335e-08</v>
+        <v>0.0003990742876771093</v>
       </c>
       <c r="F29" t="n">
-        <v>5.309629061437822e-22</v>
+        <v>0.001025866223749394</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.846969198455936e-06</v>
       </c>
     </row>
     <row r="30">
@@ -1131,20 +1266,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>0.998573212519375</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>incorrect neutral</t>
+        </is>
       </c>
       <c r="D30" t="n">
-        <v>0.0003990742876771093</v>
+        <v>0.01288723940169992</v>
       </c>
       <c r="E30" t="n">
-        <v>0.001025866223749394</v>
+        <v>0.0002606973730451644</v>
       </c>
       <c r="F30" t="n">
-        <v>1.846969198455936e-06</v>
+        <v>0.9868520632252141</v>
+      </c>
+      <c r="G30" t="n">
+        <v>4.06506964265733e-14</v>
       </c>
     </row>
     <row r="31">
@@ -1155,20 +1295,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>0.01288723940169992</v>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>incorrect happy</t>
+        </is>
       </c>
       <c r="D31" t="n">
-        <v>0.0002606973730451644</v>
+        <v>0.08144257809034104</v>
       </c>
       <c r="E31" t="n">
-        <v>0.9868520632252141</v>
+        <v>0.9185573282066218</v>
       </c>
       <c r="F31" t="n">
-        <v>4.06506964265733e-14</v>
+        <v>9.370303720305335e-08</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.309629061437822e-22</v>
       </c>
     </row>
     <row r="32">
@@ -1179,20 +1324,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>1.426009519948071e-09</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>incorrect neutral</t>
+        </is>
       </c>
       <c r="D32" t="n">
-        <v>0.8896752737063891</v>
+        <v>3.503645296559549e-05</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0001206871310782763</v>
+        <v>0.03477933168817512</v>
       </c>
       <c r="F32" t="n">
-        <v>0.110204037736523</v>
+        <v>0.9651773907415127</v>
+      </c>
+      <c r="G32" t="n">
+        <v>8.241117346439033e-06</v>
       </c>
     </row>
     <row r="33">
@@ -1203,20 +1353,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>3.503645296559549e-05</v>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D33" t="n">
-        <v>0.03477933168817512</v>
+        <v>4.014689492725665e-05</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9651773907415127</v>
+        <v>0.9986293339753848</v>
       </c>
       <c r="F33" t="n">
-        <v>8.241117346439033e-06</v>
+        <v>0.001330518332464757</v>
+      </c>
+      <c r="G33" t="n">
+        <v>7.972231476719833e-10</v>
       </c>
     </row>
     <row r="34">
@@ -1227,20 +1382,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>4.014689492725665e-05</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D34" t="n">
-        <v>0.9986293339753848</v>
+        <v>1.426009519948071e-09</v>
       </c>
       <c r="E34" t="n">
-        <v>0.001330518332464757</v>
+        <v>0.8896752737063891</v>
       </c>
       <c r="F34" t="n">
-        <v>7.972231476719833e-10</v>
+        <v>0.0001206871310782763</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.110204037736523</v>
       </c>
     </row>
     <row r="35">
@@ -1251,20 +1411,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>1.943800643359612e-08</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D35" t="n">
-        <v>4.086933765320614e-07</v>
+        <v>1.403598953564861e-09</v>
       </c>
       <c r="E35" t="n">
-        <v>0.9999995714444387</v>
+        <v>1.185882010835925e-06</v>
       </c>
       <c r="F35" t="n">
-        <v>4.241782555792451e-10</v>
+        <v>0.999987356642669</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1.145607172124487e-05</v>
       </c>
     </row>
     <row r="36">
@@ -1275,20 +1440,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>1.403598953564861e-09</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D36" t="n">
-        <v>1.185882010835925e-06</v>
+        <v>1.226635163855063e-11</v>
       </c>
       <c r="E36" t="n">
-        <v>0.999987356642669</v>
+        <v>4.884523151363319e-09</v>
       </c>
       <c r="F36" t="n">
-        <v>1.145607172124487e-05</v>
+        <v>0.9999999942280855</v>
+      </c>
+      <c r="G36" t="n">
+        <v>8.751248385225806e-10</v>
       </c>
     </row>
     <row r="37">
@@ -1299,20 +1469,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
-        <v>1.226635163855063e-11</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D37" t="n">
-        <v>4.884523151363319e-09</v>
+        <v>4.30622990737897e-10</v>
       </c>
       <c r="E37" t="n">
-        <v>0.9999999942280855</v>
+        <v>1.777424020284196e-09</v>
       </c>
       <c r="F37" t="n">
-        <v>8.751248385225806e-10</v>
+        <v>0.9999999961169608</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1.674992057146099e-09</v>
       </c>
     </row>
     <row r="38">
@@ -1323,20 +1498,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
-        <v>4.30622990737897e-10</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D38" t="n">
-        <v>1.777424020284196e-09</v>
+        <v>1.208492254400782e-12</v>
       </c>
       <c r="E38" t="n">
-        <v>0.9999999961169608</v>
+        <v>9.414490715148804e-11</v>
       </c>
       <c r="F38" t="n">
-        <v>1.674992057146099e-09</v>
+        <v>0.9999999998804396</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2.420688105771143e-11</v>
       </c>
     </row>
     <row r="39">
@@ -1347,20 +1527,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C39" t="n">
-        <v>1.208492254400782e-12</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D39" t="n">
-        <v>9.414490715148804e-11</v>
+        <v>1.943800643359612e-08</v>
       </c>
       <c r="E39" t="n">
-        <v>0.9999999998804396</v>
+        <v>4.086933765320614e-07</v>
       </c>
       <c r="F39" t="n">
-        <v>2.420688105771143e-11</v>
+        <v>0.9999995714444387</v>
+      </c>
+      <c r="G39" t="n">
+        <v>4.241782555792451e-10</v>
       </c>
     </row>
     <row r="40">
@@ -1371,20 +1556,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>incorrect neutral</t>
         </is>
       </c>
-      <c r="C40" t="n">
-        <v>6.734879062730671e-14</v>
-      </c>
       <c r="D40" t="n">
-        <v>9.296461668540372e-10</v>
+        <v>1.291918045288698e-09</v>
       </c>
       <c r="E40" t="n">
-        <v>0.999999999070041</v>
+        <v>0.0008702118631205627</v>
       </c>
       <c r="F40" t="n">
-        <v>2.454941885365347e-13</v>
+        <v>0.9962375562299454</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.002892230615016065</v>
       </c>
     </row>
     <row r="41">
@@ -1395,20 +1585,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
-        </is>
-      </c>
-      <c r="C41" t="n">
-        <v>1.291918045288698e-09</v>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D41" t="n">
-        <v>0.0008702118631205627</v>
+        <v>1.776057772770287e-14</v>
       </c>
       <c r="E41" t="n">
-        <v>0.9962375562299454</v>
+        <v>8.25256065935441e-12</v>
       </c>
       <c r="F41" t="n">
-        <v>0.002892230615016065</v>
+        <v>0.009795388217495248</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.9902046117742345</v>
       </c>
     </row>
     <row r="42">
@@ -1419,26 +1614,31 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>1.776057772770287e-14</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>incorrect neutral</t>
+        </is>
       </c>
       <c r="D42" t="n">
-        <v>8.25256065935441e-12</v>
+        <v>6.734879062730671e-14</v>
       </c>
       <c r="E42" t="n">
-        <v>0.009795388217495248</v>
+        <v>9.296461668540372e-10</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9902046117742345</v>
+        <v>0.999999999070041</v>
+      </c>
+      <c r="G42" t="n">
+        <v>2.454941885365347e-13</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>JLCorpus audio</t>
+          <t>JL audio</t>
         </is>
       </c>
     </row>
@@ -1450,19 +1650,24 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>incorrect happy</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="D44" t="n">
         <v>0.03130012115633713</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>0.9686998483356055</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>2.734056260570158e-08</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>3.167494693366019e-09</v>
       </c>
     </row>
@@ -1474,19 +1679,24 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
         <v>0.9999997658713984</v>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="n">
         <v>2.341252026837822e-07</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>3.393910339747311e-12</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>5.170899353180098e-15</v>
       </c>
     </row>
@@ -1498,19 +1708,24 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
         <v>0.9999999827512501</v>
       </c>
-      <c r="D46" t="n">
+      <c r="E46" t="n">
         <v>1.724806482086797e-08</v>
       </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
         <v>9.051858930645069e-16</v>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>6.841267732129574e-13</v>
       </c>
     </row>
@@ -1522,19 +1737,24 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C47" t="n">
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
         <v>0.9999981489438758</v>
       </c>
-      <c r="D47" t="n">
+      <c r="E47" t="n">
         <v>1.80558268397725e-06</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>4.525436208148148e-08</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>2.19078121362754e-10</v>
       </c>
     </row>
@@ -1546,20 +1766,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>incorrect happy</t>
-        </is>
-      </c>
-      <c r="C48" t="n">
-        <v>0.3618317492240281</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D48" t="n">
-        <v>0.6381648147985317</v>
+        <v>0.6473000232512405</v>
       </c>
       <c r="E48" t="n">
-        <v>2.887581080372506e-08</v>
+        <v>0.3526650346501983</v>
       </c>
       <c r="F48" t="n">
-        <v>3.407101629380745e-06</v>
+        <v>3.421237152200893e-05</v>
+      </c>
+      <c r="G48" t="n">
+        <v>7.297270392678669e-07</v>
       </c>
     </row>
     <row r="49">
@@ -1570,20 +1795,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C49" t="n">
-        <v>0.6473000232512405</v>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D49" t="n">
-        <v>0.3526650346501983</v>
+        <v>0.9999999910402356</v>
       </c>
       <c r="E49" t="n">
-        <v>3.421237152200893e-05</v>
+        <v>8.959631283248769e-09</v>
       </c>
       <c r="F49" t="n">
-        <v>7.297270392678669e-07</v>
+        <v>1.333084195262829e-13</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1.985223505090241e-18</v>
       </c>
     </row>
     <row r="50">
@@ -1594,44 +1824,54 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>0.9999999910402356</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D50" t="n">
-        <v>8.959631283248769e-09</v>
+        <v>0.999999998831099</v>
       </c>
       <c r="E50" t="n">
-        <v>1.333084195262829e-13</v>
+        <v>1.031175101648718e-09</v>
       </c>
       <c r="F50" t="n">
-        <v>1.985223505090241e-18</v>
+        <v>1.113755147489007e-10</v>
+      </c>
+      <c r="G50" t="n">
+        <v>2.635023075646463e-11</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>angry</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C51" t="n">
-        <v>0.999999998831099</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D51" t="n">
-        <v>1.031175101648718e-09</v>
+        <v>0.02352518849867759</v>
       </c>
       <c r="E51" t="n">
-        <v>1.113755147489007e-10</v>
+        <v>0.8052797140541254</v>
       </c>
       <c r="F51" t="n">
-        <v>2.635023075646463e-11</v>
+        <v>0.1711946704690515</v>
+      </c>
+      <c r="G51" t="n">
+        <v>4.269781455912076e-07</v>
       </c>
     </row>
     <row r="52">
@@ -1642,20 +1882,25 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>0.02352518849867759</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D52" t="n">
-        <v>0.8052797140541254</v>
+        <v>0.0003463831908508977</v>
       </c>
       <c r="E52" t="n">
-        <v>0.1711946704690515</v>
+        <v>0.9992461014184022</v>
       </c>
       <c r="F52" t="n">
-        <v>4.269781455912076e-07</v>
+        <v>0.0003926135806871011</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1.490181005985252e-05</v>
       </c>
     </row>
     <row r="53">
@@ -1666,20 +1911,25 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C53" t="n">
-        <v>0.0003463831908508977</v>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D53" t="n">
-        <v>0.9992461014184022</v>
+        <v>2.123056368302282e-07</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0003926135806871011</v>
+        <v>0.9999997812636404</v>
       </c>
       <c r="F53" t="n">
-        <v>1.490181005985252e-05</v>
+        <v>6.405086820697973e-09</v>
+      </c>
+      <c r="G53" t="n">
+        <v>2.56359605192664e-11</v>
       </c>
     </row>
     <row r="54">
@@ -1690,20 +1940,25 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C54" t="n">
-        <v>2.123056368302282e-07</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D54" t="n">
-        <v>0.9999997812636404</v>
+        <v>2.59625020154014e-12</v>
       </c>
       <c r="E54" t="n">
-        <v>6.405086820697973e-09</v>
+        <v>0.9999964720816381</v>
       </c>
       <c r="F54" t="n">
-        <v>2.56359605192664e-11</v>
+        <v>1.564956279207119e-09</v>
+      </c>
+      <c r="G54" t="n">
+        <v>3.526350809429424e-06</v>
       </c>
     </row>
     <row r="55">
@@ -1714,20 +1969,25 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C55" t="n">
-        <v>2.59625020154014e-12</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D55" t="n">
-        <v>0.9999964720816381</v>
+        <v>0.01471149268719845</v>
       </c>
       <c r="E55" t="n">
-        <v>1.564956279207119e-09</v>
+        <v>0.9852183119320149</v>
       </c>
       <c r="F55" t="n">
-        <v>3.526350809429424e-06</v>
+        <v>2.445873555954392e-05</v>
+      </c>
+      <c r="G55" t="n">
+        <v>4.573664522715527e-05</v>
       </c>
     </row>
     <row r="56">
@@ -1738,20 +1998,25 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C56" t="n">
-        <v>0.01471149268719845</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D56" t="n">
-        <v>0.9852183119320149</v>
+        <v>1.529380350351737e-05</v>
       </c>
       <c r="E56" t="n">
-        <v>2.445873555954392e-05</v>
+        <v>0.9999585308344019</v>
       </c>
       <c r="F56" t="n">
-        <v>4.573664522715527e-05</v>
+        <v>2.147612830633627e-05</v>
+      </c>
+      <c r="G56" t="n">
+        <v>4.699233788076977e-06</v>
       </c>
     </row>
     <row r="57">
@@ -1762,68 +2027,83 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C57" t="n">
-        <v>1.529380350351737e-05</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D57" t="n">
-        <v>0.9999585308344019</v>
+        <v>4.905694321162588e-05</v>
       </c>
       <c r="E57" t="n">
-        <v>2.147612830633627e-05</v>
+        <v>0.999879988054084</v>
       </c>
       <c r="F57" t="n">
-        <v>4.699233788076977e-06</v>
+        <v>4.651476801232238e-07</v>
+      </c>
+      <c r="G57" t="n">
+        <v>7.048985502420139e-05</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C58" t="n">
-        <v>7.346427186821857e-05</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D58" t="n">
-        <v>0.9985984970367721</v>
+        <v>0.03932102878316885</v>
       </c>
       <c r="E58" t="n">
-        <v>0.001327931537802398</v>
+        <v>0.04157180779323957</v>
       </c>
       <c r="F58" t="n">
-        <v>1.071535573377898e-07</v>
+        <v>0.91879472569947</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.0003124377241216265</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C59" t="n">
-        <v>4.905694321162588e-05</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D59" t="n">
-        <v>0.999879988054084</v>
+        <v>1.521476539800239e-07</v>
       </c>
       <c r="E59" t="n">
-        <v>4.651476801232238e-07</v>
+        <v>0.0008487881057721555</v>
       </c>
       <c r="F59" t="n">
-        <v>7.048985502420139e-05</v>
+        <v>0.8686793674612773</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.1304716922852966</v>
       </c>
     </row>
     <row r="60">
@@ -1834,20 +2114,25 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C60" t="n">
-        <v>0.03932102878316885</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D60" t="n">
-        <v>0.04157180779323957</v>
+        <v>9.966631207651111e-07</v>
       </c>
       <c r="E60" t="n">
-        <v>0.91879472569947</v>
+        <v>2.57942715782938e-10</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0003124377241216265</v>
+        <v>0.9991191509556385</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.0008798521232979835</v>
       </c>
     </row>
     <row r="61">
@@ -1858,20 +2143,25 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C61" t="n">
-        <v>1.521476539800239e-07</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D61" t="n">
-        <v>0.0008487881057721555</v>
+        <v>1.224690534897892e-10</v>
       </c>
       <c r="E61" t="n">
-        <v>0.8686793674612773</v>
+        <v>3.122577511005219e-06</v>
       </c>
       <c r="F61" t="n">
-        <v>0.1304716922852966</v>
+        <v>0.9999968703159957</v>
+      </c>
+      <c r="G61" t="n">
+        <v>6.984024218849883e-09</v>
       </c>
     </row>
     <row r="62">
@@ -1882,20 +2172,25 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C62" t="n">
-        <v>9.966631207651111e-07</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D62" t="n">
-        <v>2.57942715782938e-10</v>
+        <v>7.511285807726668e-07</v>
       </c>
       <c r="E62" t="n">
-        <v>0.9991191509556385</v>
+        <v>2.141678864751088e-05</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0008798521232979835</v>
+        <v>0.9914557949143274</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.008522037168444452</v>
       </c>
     </row>
     <row r="63">
@@ -1906,20 +2201,25 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C63" t="n">
-        <v>1.224690534897892e-10</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D63" t="n">
-        <v>3.122577511005219e-06</v>
+        <v>2.361907307238748e-07</v>
       </c>
       <c r="E63" t="n">
-        <v>0.9999968703159957</v>
+        <v>0.01233680889919175</v>
       </c>
       <c r="F63" t="n">
-        <v>6.984024218849883e-09</v>
+        <v>0.9677950749510463</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.01986787995903112</v>
       </c>
     </row>
     <row r="64">
@@ -1930,20 +2230,25 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C64" t="n">
-        <v>7.511285807726668e-07</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D64" t="n">
-        <v>2.141678864751088e-05</v>
+        <v>7.915490148003956e-08</v>
       </c>
       <c r="E64" t="n">
-        <v>0.9914557949143274</v>
+        <v>0.002238612454534579</v>
       </c>
       <c r="F64" t="n">
-        <v>0.008522037168444452</v>
+        <v>0.997732986094622</v>
+      </c>
+      <c r="G64" t="n">
+        <v>2.832229594211349e-05</v>
       </c>
     </row>
     <row r="65">
@@ -1954,68 +2259,83 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C65" t="n">
-        <v>2.361907307238748e-07</v>
+          <t>med</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D65" t="n">
-        <v>0.01233680889919175</v>
+        <v>1.49917375319637e-08</v>
       </c>
       <c r="E65" t="n">
-        <v>0.9677950749510463</v>
+        <v>0.000278967735139921</v>
       </c>
       <c r="F65" t="n">
-        <v>0.01986787995903112</v>
+        <v>0.984674273297942</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.01504674397518064</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>sad</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C66" t="n">
-        <v>7.915490148003956e-08</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>incorrect neutral</t>
+        </is>
       </c>
       <c r="D66" t="n">
-        <v>0.002238612454534579</v>
+        <v>0.003920491024751745</v>
       </c>
       <c r="E66" t="n">
-        <v>0.997732986094622</v>
+        <v>0.00347523334142926</v>
       </c>
       <c r="F66" t="n">
-        <v>2.832229594211349e-05</v>
+        <v>0.7880747211989104</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.2045295544349086</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>sad</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C67" t="n">
-        <v>1.49917375319637e-08</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>incorrect angry</t>
+        </is>
       </c>
       <c r="D67" t="n">
-        <v>0.000278967735139921</v>
+        <v>0.9552573600481038</v>
       </c>
       <c r="E67" t="n">
-        <v>0.984674273297942</v>
+        <v>0.01081141247446618</v>
       </c>
       <c r="F67" t="n">
-        <v>0.01504674397518064</v>
+        <v>0.02130369864989802</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.01262752882753212</v>
       </c>
     </row>
     <row r="68">
@@ -2026,20 +2346,25 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
-        </is>
-      </c>
-      <c r="C68" t="n">
-        <v>0.003920491024751745</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D68" t="n">
-        <v>0.00347523334142926</v>
+        <v>0.0004724475040417419</v>
       </c>
       <c r="E68" t="n">
-        <v>0.7880747211989104</v>
+        <v>0.2341160541966946</v>
       </c>
       <c r="F68" t="n">
-        <v>0.2045295544349086</v>
+        <v>0.0005458520238284552</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.7648656462754353</v>
       </c>
     </row>
     <row r="69">
@@ -2050,20 +2375,25 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
-        </is>
-      </c>
-      <c r="C69" t="n">
-        <v>0.9552573600481038</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D69" t="n">
-        <v>0.01081141247446618</v>
+        <v>1.933608171592541e-10</v>
       </c>
       <c r="E69" t="n">
-        <v>0.02130369864989802</v>
+        <v>1.872458002424772e-07</v>
       </c>
       <c r="F69" t="n">
-        <v>0.01262752882753212</v>
+        <v>0.0001835745500298561</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.999816238010809</v>
       </c>
     </row>
     <row r="70">
@@ -2074,20 +2404,25 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C70" t="n">
-        <v>0.0004724475040417419</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D70" t="n">
-        <v>0.2341160541966946</v>
+        <v>2.026604839931455e-12</v>
       </c>
       <c r="E70" t="n">
-        <v>0.0005458520238284552</v>
+        <v>0.0002849758667794369</v>
       </c>
       <c r="F70" t="n">
-        <v>0.7648656462754353</v>
+        <v>1.447478911737849e-05</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.9997005493420765</v>
       </c>
     </row>
     <row r="71">
@@ -2098,115 +2433,24 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C71" t="n">
-        <v>3.143042894919002e-07</v>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
       </c>
       <c r="D71" t="n">
-        <v>1.834940301789438e-05</v>
+        <v>3.227199690806363e-15</v>
       </c>
       <c r="E71" t="n">
-        <v>9.127923542763181e-05</v>
+        <v>1.143435977244247e-06</v>
       </c>
       <c r="F71" t="n">
-        <v>0.9998900570572651</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>sad</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C72" t="n">
-        <v>0.003251279397865645</v>
-      </c>
-      <c r="D72" t="n">
-        <v>0.1378267186833491</v>
-      </c>
-      <c r="E72" t="n">
-        <v>0.001521496953566769</v>
-      </c>
-      <c r="F72" t="n">
-        <v>0.8574005049652186</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>sad</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C73" t="n">
-        <v>1.933608171592541e-10</v>
-      </c>
-      <c r="D73" t="n">
-        <v>1.872458002424772e-07</v>
-      </c>
-      <c r="E73" t="n">
-        <v>0.0001835745500298561</v>
-      </c>
-      <c r="F73" t="n">
-        <v>0.999816238010809</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>sad</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C74" t="n">
-        <v>2.026604839931455e-12</v>
-      </c>
-      <c r="D74" t="n">
-        <v>0.0002849758667794369</v>
-      </c>
-      <c r="E74" t="n">
-        <v>1.447478911737849e-05</v>
-      </c>
-      <c r="F74" t="n">
-        <v>0.9997005493420765</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>sad</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>correct</t>
-        </is>
-      </c>
-      <c r="C75" t="n">
-        <v>3.227199690806363e-15</v>
-      </c>
-      <c r="D75" t="n">
-        <v>1.143435977244247e-06</v>
-      </c>
-      <c r="E75" t="n">
         <v>0.0002687121545531161</v>
       </c>
-      <c r="F75" t="n">
+      <c r="G71" t="n">
         <v>0.9997301444094664</v>
       </c>
     </row>

</xml_diff>

<commit_message>
retrain JL with more audio data
</commit_message>
<xml_diff>
--- a/predict_from_audio/prediction.xlsx
+++ b/predict_from_audio/prediction.xlsx
@@ -514,16 +514,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.9999999999999958</v>
+        <v>0.9999999999998206</v>
       </c>
       <c r="E3" t="n">
-        <v>4.291842971261001e-15</v>
+        <v>1.793703060261124e-13</v>
       </c>
       <c r="F3" t="n">
-        <v>6.664850240386784e-26</v>
+        <v>2.056398946532721e-20</v>
       </c>
       <c r="G3" t="n">
-        <v>3.548516083498005e-31</v>
+        <v>6.122445952525272e-17</v>
       </c>
     </row>
     <row r="4">
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.9999999999948537</v>
+        <v>0.9999054226132826</v>
       </c>
       <c r="E4" t="n">
-        <v>5.14632371936683e-12</v>
+        <v>9.457738632051404e-05</v>
       </c>
       <c r="F4" t="n">
-        <v>2.810826604628501e-30</v>
+        <v>1.549260899728222e-16</v>
       </c>
       <c r="G4" t="n">
-        <v>5.268669126645495e-29</v>
+        <v>3.966572070466853e-13</v>
       </c>
     </row>
     <row r="5">
@@ -572,16 +572,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.1028776479987695</v>
+        <v>0.02052927009854033</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8529392593047024</v>
+        <v>0.8856796186149773</v>
       </c>
       <c r="F5" t="n">
-        <v>5.034413963289978e-10</v>
+        <v>1.11238966125822e-08</v>
       </c>
       <c r="G5" t="n">
-        <v>0.04418309219308678</v>
+        <v>0.09379110016258566</v>
       </c>
     </row>
     <row r="6">
@@ -601,16 +601,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.7666619846240529</v>
+        <v>0.9447287462537832</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2333361249117024</v>
+        <v>0.05449793858376263</v>
       </c>
       <c r="F6" t="n">
-        <v>1.753676013201202e-08</v>
+        <v>1.142455633691876e-09</v>
       </c>
       <c r="G6" t="n">
-        <v>1.872927484720959e-06</v>
+        <v>0.0007733140199984078</v>
       </c>
     </row>
     <row r="7">
@@ -630,16 +630,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.9999999805451004</v>
+        <v>0.999987067932688</v>
       </c>
       <c r="E7" t="n">
-        <v>1.730659591717027e-08</v>
+        <v>1.290762816805327e-05</v>
       </c>
       <c r="F7" t="n">
-        <v>4.379234582466622e-16</v>
+        <v>8.100998641643466e-12</v>
       </c>
       <c r="G7" t="n">
-        <v>2.148303320605434e-09</v>
+        <v>2.443104291797293e-08</v>
       </c>
     </row>
     <row r="8">
@@ -659,16 +659,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.9999999999994669</v>
       </c>
       <c r="E8" t="n">
-        <v>1.924163094106687e-17</v>
+        <v>5.332374964086666e-13</v>
       </c>
       <c r="F8" t="n">
-        <v>2.294331317352309e-25</v>
+        <v>5.844529150480256e-18</v>
       </c>
       <c r="G8" t="n">
-        <v>2.205737420865212e-20</v>
+        <v>2.080779671753602e-17</v>
       </c>
     </row>
     <row r="9">
@@ -688,16 +688,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7.160065647899298e-05</v>
+        <v>4.587604177440284e-06</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9938371079189601</v>
+        <v>0.9270392272039764</v>
       </c>
       <c r="F9" t="n">
-        <v>4.65572354961423e-12</v>
+        <v>1.330735789137088e-12</v>
       </c>
       <c r="G9" t="n">
-        <v>0.006091291419905157</v>
+        <v>0.07295618519051536</v>
       </c>
     </row>
     <row r="10">
@@ -717,16 +717,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>7.76776830632744e-11</v>
+        <v>8.088827760219333e-06</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9998186785052253</v>
+        <v>0.9197832810109792</v>
       </c>
       <c r="F10" t="n">
-        <v>3.704338495668053e-10</v>
+        <v>1.013798858823988e-09</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0001813210466630926</v>
+        <v>0.08020862914746167</v>
       </c>
     </row>
     <row r="11">
@@ -746,16 +746,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.0002001984622143036</v>
+        <v>0.000206415055028952</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9997988593891605</v>
+        <v>0.9997652346752788</v>
       </c>
       <c r="F11" t="n">
-        <v>3.891110493725258e-10</v>
+        <v>2.263497132374649e-10</v>
       </c>
       <c r="G11" t="n">
-        <v>9.417595141867981e-07</v>
+        <v>2.83500433425639e-05</v>
       </c>
     </row>
     <row r="12">
@@ -775,16 +775,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7.285876219785999e-05</v>
+        <v>0.001190433455649084</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9998972816148425</v>
+        <v>0.9974317891202629</v>
       </c>
       <c r="F12" t="n">
-        <v>6.163822819796504e-11</v>
+        <v>8.243540337820944e-11</v>
       </c>
       <c r="G12" t="n">
-        <v>2.985956132138134e-05</v>
+        <v>0.00137777734165259</v>
       </c>
     </row>
     <row r="13">
@@ -804,16 +804,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.000194165906865547</v>
+        <v>0.0002307609579212306</v>
       </c>
       <c r="E13" t="n">
-        <v>0.8853090716768269</v>
+        <v>0.9755314213462919</v>
       </c>
       <c r="F13" t="n">
-        <v>8.21105226983515e-10</v>
+        <v>5.361960741428253e-10</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1144967615952024</v>
+        <v>0.02423781715959066</v>
       </c>
     </row>
     <row r="14">
@@ -829,20 +829,20 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect angry</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.001205930498838876</v>
+        <v>0.8056831276577465</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9987940149404769</v>
+        <v>0.1943055264528333</v>
       </c>
       <c r="F14" t="n">
-        <v>5.321849076428152e-08</v>
+        <v>1.131113785440722e-05</v>
       </c>
       <c r="G14" t="n">
-        <v>1.342193635572525e-09</v>
+        <v>3.475156565266872e-08</v>
       </c>
     </row>
     <row r="15">
@@ -862,16 +862,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3.655756462221376e-08</v>
+        <v>4.333086847282703e-07</v>
       </c>
       <c r="E15" t="n">
-        <v>2.577857251276227e-10</v>
+        <v>0.0001462365040957021</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9999124400529332</v>
+        <v>0.9997456210930945</v>
       </c>
       <c r="G15" t="n">
-        <v>8.752313171645299e-05</v>
+        <v>0.0001077090941249973</v>
       </c>
     </row>
     <row r="16">
@@ -891,16 +891,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2.972500553988441e-13</v>
+        <v>1.654410389104317e-11</v>
       </c>
       <c r="E16" t="n">
-        <v>7.48370197481234e-13</v>
+        <v>8.180157526356826e-10</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9999999926922711</v>
+        <v>0.9999499918149986</v>
       </c>
       <c r="G16" t="n">
-        <v>7.306683243709039e-09</v>
+        <v>5.000735044163247e-05</v>
       </c>
     </row>
     <row r="17">
@@ -920,16 +920,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1.818329568804131e-09</v>
+        <v>2.018528758480901e-10</v>
       </c>
       <c r="E17" t="n">
-        <v>1.888643063654962e-07</v>
+        <v>7.02649505083139e-11</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9999789101142096</v>
+        <v>0.9996303108858972</v>
       </c>
       <c r="G17" t="n">
-        <v>2.089920315448475e-05</v>
+        <v>0.000369688841985034</v>
       </c>
     </row>
     <row r="18">
@@ -945,20 +945,20 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect sad</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.0006363948495867508</v>
+        <v>2.907073662735093e-05</v>
       </c>
       <c r="E18" t="n">
-        <v>5.097941515259609e-07</v>
+        <v>4.498325798161879e-10</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7139563691653532</v>
+        <v>0.001809629478606713</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2854067261909086</v>
+        <v>0.9981612993349332</v>
       </c>
     </row>
     <row r="19">
@@ -978,16 +978,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.0003172681374546574</v>
+        <v>0.003466848067807468</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0001624648402944739</v>
+        <v>0.0447967482774116</v>
       </c>
       <c r="F19" t="n">
-        <v>0.04522190705770469</v>
+        <v>0.0136955100517412</v>
       </c>
       <c r="G19" t="n">
-        <v>0.9542983599645463</v>
+        <v>0.9380408936030397</v>
       </c>
     </row>
     <row r="20">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>5.545270367277377e-28</v>
+        <v>6.91505193129059e-18</v>
       </c>
       <c r="E20" t="n">
-        <v>1.463973987889115e-19</v>
+        <v>4.789101935374194e-12</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>0.9999999999952109</v>
       </c>
       <c r="G20" t="n">
-        <v>3.175281052112876e-27</v>
+        <v>4.728619417665846e-20</v>
       </c>
     </row>
     <row r="21">
@@ -1036,16 +1036,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.002231699238719564</v>
+        <v>0.08005789202850304</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9974179253866701</v>
+        <v>0.7305389157737315</v>
       </c>
       <c r="F21" t="n">
-        <v>5.738168981725291e-08</v>
+        <v>0.0004424259379489041</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0003503179929204975</v>
+        <v>0.1889607662598164</v>
       </c>
     </row>
     <row r="22">
@@ -1065,16 +1065,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1.385949479775801e-11</v>
+        <v>9.875551766673574e-11</v>
       </c>
       <c r="E22" t="n">
-        <v>2.655397194628444e-06</v>
+        <v>0.000491140788611244</v>
       </c>
       <c r="F22" t="n">
-        <v>1.321731236149002e-13</v>
+        <v>1.019442431792011e-13</v>
       </c>
       <c r="G22" t="n">
-        <v>0.9999973445888137</v>
+        <v>0.9995088591125313</v>
       </c>
     </row>
     <row r="23">
@@ -1094,16 +1094,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>2.754138719955606e-08</v>
+        <v>3.252361631904944e-06</v>
       </c>
       <c r="E23" t="n">
-        <v>2.950762256335242e-09</v>
+        <v>6.422429954005728e-06</v>
       </c>
       <c r="F23" t="n">
-        <v>7.758747690774755e-08</v>
+        <v>2.658756050152348e-07</v>
       </c>
       <c r="G23" t="n">
-        <v>0.9999998919203735</v>
+        <v>0.999990059332809</v>
       </c>
     </row>
     <row r="24">
@@ -1123,16 +1123,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>7.933797805376025e-08</v>
+        <v>7.569535044712422e-08</v>
       </c>
       <c r="E24" t="n">
-        <v>2.964556447554696e-06</v>
+        <v>0.0001739156785718625</v>
       </c>
       <c r="F24" t="n">
-        <v>0.00266459986949977</v>
+        <v>5.276613380130639e-07</v>
       </c>
       <c r="G24" t="n">
-        <v>0.9973323562360746</v>
+        <v>0.9998254809647396</v>
       </c>
     </row>
     <row r="25">
@@ -1152,16 +1152,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.001097363121574919</v>
+        <v>0.0007360686196491984</v>
       </c>
       <c r="E25" t="n">
-        <v>5.848600996144805e-06</v>
+        <v>0.04887448219268421</v>
       </c>
       <c r="F25" t="n">
-        <v>1.842475169408814e-07</v>
+        <v>6.770073877701122e-07</v>
       </c>
       <c r="G25" t="n">
-        <v>0.998896604029912</v>
+        <v>0.9503887721802788</v>
       </c>
     </row>
     <row r="26">
@@ -1181,16 +1181,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.002279360278761463</v>
+        <v>0.003796137349295674</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0006771214237469849</v>
+        <v>0.0001367020271562012</v>
       </c>
       <c r="F26" t="n">
-        <v>1.563430323446e-10</v>
+        <v>4.665248123481654e-12</v>
       </c>
       <c r="G26" t="n">
-        <v>0.9970435181411484</v>
+        <v>0.9960671606188828</v>
       </c>
     </row>
     <row r="27">
@@ -1210,16 +1210,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1.059520242209503e-08</v>
+        <v>2.503830043952667e-12</v>
       </c>
       <c r="E27" t="n">
-        <v>0.001041189892020689</v>
+        <v>1.001033485617876e-06</v>
       </c>
       <c r="F27" t="n">
-        <v>3.398143805496473e-05</v>
+        <v>2.576038604339349e-08</v>
       </c>
       <c r="G27" t="n">
-        <v>0.9989248180747219</v>
+        <v>0.9999989732036245</v>
       </c>
     </row>
     <row r="28">
@@ -1242,20 +1242,20 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.9985138950932791</v>
+        <v>0.01658336940832141</v>
       </c>
       <c r="E29" t="n">
-        <v>0.001395457365251516</v>
+        <v>0.02965725824107039</v>
       </c>
       <c r="F29" t="n">
-        <v>9.002226007585246e-05</v>
+        <v>0.9535519153446452</v>
       </c>
       <c r="G29" t="n">
-        <v>6.25281393438542e-07</v>
+        <v>0.0002074570059630105</v>
       </c>
     </row>
     <row r="30">
@@ -1271,20 +1271,20 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.9821838436615558</v>
+        <v>0.01214384062878948</v>
       </c>
       <c r="E30" t="n">
-        <v>0.01527317416698585</v>
+        <v>0.0001045257048271933</v>
       </c>
       <c r="F30" t="n">
-        <v>0.002542982170915214</v>
+        <v>0.9877516336410835</v>
       </c>
       <c r="G30" t="n">
-        <v>5.432284171156349e-13</v>
+        <v>2.529972791643732e-11</v>
       </c>
     </row>
     <row r="31">
@@ -1304,16 +1304,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.9732081991621836</v>
+        <v>0.9911224215496567</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0267869025117782</v>
+        <v>0.008196723033411917</v>
       </c>
       <c r="F31" t="n">
-        <v>4.898326032057085e-06</v>
+        <v>0.000680855416917874</v>
       </c>
       <c r="G31" t="n">
-        <v>6.355023023028633e-15</v>
+        <v>1.347648689779427e-14</v>
       </c>
     </row>
     <row r="32">
@@ -1329,20 +1329,20 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.0006386043817762741</v>
+        <v>2.653118030088392e-05</v>
       </c>
       <c r="E32" t="n">
-        <v>0.981296369090792</v>
+        <v>0.005434232738071854</v>
       </c>
       <c r="F32" t="n">
-        <v>9.031154649543065e-05</v>
+        <v>0.9829768959633907</v>
       </c>
       <c r="G32" t="n">
-        <v>0.01797471498093638</v>
+        <v>0.01156234011823653</v>
       </c>
     </row>
     <row r="33">
@@ -1358,20 +1358,20 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1.956359993844653e-05</v>
+        <v>0.0001266898983563425</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9996685104315433</v>
+        <v>0.4366818287920385</v>
       </c>
       <c r="F33" t="n">
-        <v>0.0003119259674572739</v>
+        <v>0.5631914813083059</v>
       </c>
       <c r="G33" t="n">
-        <v>1.061000760452213e-12</v>
+        <v>1.299224069565445e-12</v>
       </c>
     </row>
     <row r="34">
@@ -1387,20 +1387,20 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4.839759287479072e-11</v>
+        <v>1.479045745096434e-06</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9476002683891231</v>
+        <v>0.1816386703201291</v>
       </c>
       <c r="F34" t="n">
-        <v>1.039938239568582e-06</v>
+        <v>0.6738467433487805</v>
       </c>
       <c r="G34" t="n">
-        <v>0.05239869162423963</v>
+        <v>0.1445131072853452</v>
       </c>
     </row>
     <row r="35">
@@ -1420,16 +1420,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2.277879958525259e-07</v>
+        <v>1.268633169619202e-09</v>
       </c>
       <c r="E35" t="n">
-        <v>0.002553840301145668</v>
+        <v>1.622818759657926e-05</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9973362790902925</v>
+        <v>0.759662234104063</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0001096528205658584</v>
+        <v>0.2403215364397074</v>
       </c>
     </row>
     <row r="36">
@@ -1449,16 +1449,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2.022313995417564e-07</v>
+        <v>3.053533370936658e-10</v>
       </c>
       <c r="E36" t="n">
-        <v>0.0003685638588346244</v>
+        <v>1.533033100217406e-05</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9996253983962692</v>
+        <v>0.9999827699929185</v>
       </c>
       <c r="G36" t="n">
-        <v>5.835513496658163e-06</v>
+        <v>1.899370726013014e-06</v>
       </c>
     </row>
     <row r="37">
@@ -1478,16 +1478,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>5.707501683432479e-05</v>
+        <v>6.911721793948934e-07</v>
       </c>
       <c r="E37" t="n">
-        <v>1.261961929844891e-05</v>
+        <v>0.0001206507765159438</v>
       </c>
       <c r="F37" t="n">
-        <v>0.9998965061965462</v>
+        <v>0.999633864121422</v>
       </c>
       <c r="G37" t="n">
-        <v>3.379916732096168e-05</v>
+        <v>0.0002447939298826947</v>
       </c>
     </row>
     <row r="38">
@@ -1507,16 +1507,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.0006155126132738892</v>
+        <v>3.418393327004605e-09</v>
       </c>
       <c r="E38" t="n">
-        <v>0.002993572345217918</v>
+        <v>4.403112394161506e-07</v>
       </c>
       <c r="F38" t="n">
-        <v>0.9963903223233888</v>
+        <v>0.9999995521827481</v>
       </c>
       <c r="G38" t="n">
-        <v>5.927181194405319e-07</v>
+        <v>4.087619019929378e-09</v>
       </c>
     </row>
     <row r="39">
@@ -1536,16 +1536,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>3.31732578050885e-09</v>
+        <v>3.151436846641095e-07</v>
       </c>
       <c r="E39" t="n">
-        <v>0.007827375525017551</v>
+        <v>0.008930395866950044</v>
       </c>
       <c r="F39" t="n">
-        <v>0.9921725371939109</v>
+        <v>0.9827268808048482</v>
       </c>
       <c r="G39" t="n">
-        <v>8.396374569849997e-08</v>
+        <v>0.00834240818451721</v>
       </c>
     </row>
     <row r="40">
@@ -1561,20 +1561,20 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.9717799913671447</v>
+        <v>3.706734019076029e-10</v>
       </c>
       <c r="E40" t="n">
-        <v>0.001300774395927988</v>
+        <v>0.001214128097540298</v>
       </c>
       <c r="F40" t="n">
-        <v>0.02691406198559396</v>
+        <v>0.9987826056017725</v>
       </c>
       <c r="G40" t="n">
-        <v>5.172251333360694e-06</v>
+        <v>3.265930013849625e-06</v>
       </c>
     </row>
     <row r="41">
@@ -1590,20 +1590,20 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect neutral</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.0004977798907468674</v>
+        <v>4.37754810229941e-12</v>
       </c>
       <c r="E41" t="n">
-        <v>5.142361763322649e-05</v>
+        <v>5.137366038245314e-06</v>
       </c>
       <c r="F41" t="n">
-        <v>0.00553142733123216</v>
+        <v>0.9943169680039825</v>
       </c>
       <c r="G41" t="n">
-        <v>0.9939193691603877</v>
+        <v>0.00567789462560152</v>
       </c>
     </row>
     <row r="42">
@@ -1623,16 +1623,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>3.444715037311226e-12</v>
+        <v>4.963941540497024e-13</v>
       </c>
       <c r="E42" t="n">
-        <v>7.496683463678375e-10</v>
+        <v>1.923931072837189e-06</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9999999992356097</v>
+        <v>0.9999980689574653</v>
       </c>
       <c r="G42" t="n">
-        <v>1.127709174122137e-11</v>
+        <v>7.110965467416398e-09</v>
       </c>
     </row>
     <row r="43">
@@ -1655,20 +1655,20 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect happy</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.9999990763141896</v>
+        <v>0.02424401979475163</v>
       </c>
       <c r="E44" t="n">
-        <v>9.206552897223325e-07</v>
+        <v>0.9757015196876555</v>
       </c>
       <c r="F44" t="n">
-        <v>2.895862454904281e-09</v>
+        <v>1.993399304549397e-05</v>
       </c>
       <c r="G44" t="n">
-        <v>1.346581505253812e-10</v>
+        <v>3.452652454731885e-05</v>
       </c>
     </row>
     <row r="45">
@@ -1688,16 +1688,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.9995721707214061</v>
+        <v>0.9999963794878761</v>
       </c>
       <c r="E45" t="n">
-        <v>0.0004277051603969974</v>
+        <v>3.612101838992725e-06</v>
       </c>
       <c r="F45" t="n">
-        <v>1.240793965796923e-07</v>
+        <v>8.38225421385483e-09</v>
       </c>
       <c r="G45" t="n">
-        <v>3.880030766790171e-11</v>
+        <v>2.80305726067088e-11</v>
       </c>
     </row>
     <row r="46">
@@ -1717,16 +1717,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.9539258483916849</v>
+        <v>0.9987931821755892</v>
       </c>
       <c r="E46" t="n">
-        <v>0.04607404132146721</v>
+        <v>0.001206808416039201</v>
       </c>
       <c r="F46" t="n">
-        <v>2.526943550558931e-11</v>
+        <v>1.380651749057283e-09</v>
       </c>
       <c r="G46" t="n">
-        <v>1.102615785434258e-07</v>
+        <v>8.02771963553808e-09</v>
       </c>
     </row>
     <row r="47">
@@ -1746,16 +1746,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.9999981530171983</v>
+        <v>0.999998613024392</v>
       </c>
       <c r="E47" t="n">
-        <v>5.841944121847604e-07</v>
+        <v>1.380498956921075e-06</v>
       </c>
       <c r="F47" t="n">
-        <v>1.271615726920332e-09</v>
+        <v>4.978686331213217e-09</v>
       </c>
       <c r="G47" t="n">
-        <v>1.26151677394715e-06</v>
+        <v>1.497964835154331e-09</v>
       </c>
     </row>
     <row r="48">
@@ -1771,20 +1771,20 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>incorrect happy</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.007871791400733479</v>
+        <v>0.9232988364624176</v>
       </c>
       <c r="E48" t="n">
-        <v>0.6128757529131004</v>
+        <v>0.06862012298908288</v>
       </c>
       <c r="F48" t="n">
-        <v>0.0001185916241580908</v>
+        <v>0.003252071817725817</v>
       </c>
       <c r="G48" t="n">
-        <v>0.3791338640620082</v>
+        <v>0.004828968730773915</v>
       </c>
     </row>
     <row r="49">
@@ -1800,20 +1800,20 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.2332444962664054</v>
+        <v>0.9999999642080148</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0003675827653404404</v>
+        <v>3.235488931177493e-08</v>
       </c>
       <c r="F49" t="n">
-        <v>0.7663867206818044</v>
+        <v>3.436913455728124e-09</v>
       </c>
       <c r="G49" t="n">
-        <v>1.20028644976747e-06</v>
+        <v>1.822078852702967e-13</v>
       </c>
     </row>
     <row r="50">
@@ -1829,20 +1829,20 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>6.551752050482521e-07</v>
+        <v>0.9999574618360297</v>
       </c>
       <c r="E50" t="n">
-        <v>1.356955454948891e-09</v>
+        <v>3.667483034711684e-05</v>
       </c>
       <c r="F50" t="n">
-        <v>0.9999993434677279</v>
+        <v>5.85478660141948e-06</v>
       </c>
       <c r="G50" t="n">
-        <v>1.113762688978389e-13</v>
+        <v>8.547021758034101e-09</v>
       </c>
     </row>
     <row r="51">
@@ -1858,20 +1858,20 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.9987928470289754</v>
+        <v>0.001793372745092494</v>
       </c>
       <c r="E51" t="n">
-        <v>0.001131361931589145</v>
+        <v>0.9582655907252511</v>
       </c>
       <c r="F51" t="n">
-        <v>7.528197393809798e-05</v>
+        <v>0.03990108406703404</v>
       </c>
       <c r="G51" t="n">
-        <v>5.090654972002815e-07</v>
+        <v>3.995246262221985e-05</v>
       </c>
     </row>
     <row r="52">
@@ -1887,20 +1887,20 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.007409030347535253</v>
+        <v>0.0008400150397494511</v>
       </c>
       <c r="E52" t="n">
-        <v>0.03906469647204787</v>
+        <v>0.5842192767916078</v>
       </c>
       <c r="F52" t="n">
-        <v>0.02094113744760194</v>
+        <v>0.05632199283303619</v>
       </c>
       <c r="G52" t="n">
-        <v>0.9325851357328149</v>
+        <v>0.3586187153356064</v>
       </c>
     </row>
     <row r="53">
@@ -1920,16 +1920,16 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.004799249208770575</v>
+        <v>3.879121929617445e-06</v>
       </c>
       <c r="E53" t="n">
-        <v>0.9817976587631646</v>
+        <v>0.9993774501022757</v>
       </c>
       <c r="F53" t="n">
-        <v>6.438451510797853e-05</v>
+        <v>0.0002522313349106097</v>
       </c>
       <c r="G53" t="n">
-        <v>0.01333870751295684</v>
+        <v>0.0003664394408839803</v>
       </c>
     </row>
     <row r="54">
@@ -1945,20 +1945,20 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>1.598103641043612e-08</v>
+        <v>0.0001878365051234543</v>
       </c>
       <c r="E54" t="n">
-        <v>0.008761165132780611</v>
+        <v>0.89566229587406</v>
       </c>
       <c r="F54" t="n">
-        <v>1.242975827326497e-06</v>
+        <v>0.0001184380971116779</v>
       </c>
       <c r="G54" t="n">
-        <v>0.9912375759103557</v>
+        <v>0.1040314295237048</v>
       </c>
     </row>
     <row r="55">
@@ -1974,20 +1974,20 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.9999339846254708</v>
+        <v>0.01612548823391113</v>
       </c>
       <c r="E55" t="n">
-        <v>3.391344941872646e-05</v>
+        <v>0.9724377956660167</v>
       </c>
       <c r="F55" t="n">
-        <v>3.09874852867033e-05</v>
+        <v>0.003750878566054871</v>
       </c>
       <c r="G55" t="n">
-        <v>1.114439823899813e-06</v>
+        <v>0.007685837534017256</v>
       </c>
     </row>
     <row r="56">
@@ -2003,20 +2003,20 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.9815260573505181</v>
+        <v>0.000146300065436307</v>
       </c>
       <c r="E56" t="n">
-        <v>0.01842195102501501</v>
+        <v>0.9988585336248489</v>
       </c>
       <c r="F56" t="n">
-        <v>1.301743623023468e-05</v>
+        <v>0.0001729126475869642</v>
       </c>
       <c r="G56" t="n">
-        <v>3.897418823664729e-05</v>
+        <v>0.000822253662127893</v>
       </c>
     </row>
     <row r="57">
@@ -2032,20 +2032,20 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.9670289070690465</v>
+        <v>0.0005473406769234696</v>
       </c>
       <c r="E57" t="n">
-        <v>0.02920779425810329</v>
+        <v>0.9928162393794167</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0003877147067739142</v>
+        <v>0.001817297255893599</v>
       </c>
       <c r="G57" t="n">
-        <v>0.003375583966076141</v>
+        <v>0.004819122687766376</v>
       </c>
     </row>
     <row r="58">
@@ -2061,20 +2061,20 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.9597341528934624</v>
+        <v>0.002115686025021834</v>
       </c>
       <c r="E58" t="n">
-        <v>0.03464899927690934</v>
+        <v>0.272987841598359</v>
       </c>
       <c r="F58" t="n">
-        <v>0.001456499090789245</v>
+        <v>0.7128532053207818</v>
       </c>
       <c r="G58" t="n">
-        <v>0.004160348738838881</v>
+        <v>0.01204326705583719</v>
       </c>
     </row>
     <row r="59">
@@ -2090,20 +2090,20 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>correct</t>
+          <t>incorrect sad</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>1.886443638876253e-08</v>
+        <v>1.60268114014748e-05</v>
       </c>
       <c r="E59" t="n">
-        <v>0.0727365917750548</v>
+        <v>0.0002226418470873795</v>
       </c>
       <c r="F59" t="n">
-        <v>0.6959178305702619</v>
+        <v>0.1710051997406683</v>
       </c>
       <c r="G59" t="n">
-        <v>0.231345558790247</v>
+        <v>0.8287561316008429</v>
       </c>
     </row>
     <row r="60">
@@ -2119,20 +2119,20 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>incorrect happy</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>1.313338300094675e-05</v>
+        <v>9.297747259372726e-06</v>
       </c>
       <c r="E60" t="n">
-        <v>0.7244059180929849</v>
+        <v>2.32425207969141e-05</v>
       </c>
       <c r="F60" t="n">
-        <v>0.2507082824937121</v>
+        <v>0.9918064605490474</v>
       </c>
       <c r="G60" t="n">
-        <v>0.02487266603030205</v>
+        <v>0.008160999182896228</v>
       </c>
     </row>
     <row r="61">
@@ -2152,16 +2152,16 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.001534787216729833</v>
+        <v>5.131369128587483e-06</v>
       </c>
       <c r="E61" t="n">
-        <v>0.3044129759117679</v>
+        <v>3.606081104231401e-06</v>
       </c>
       <c r="F61" t="n">
-        <v>0.5033204456688634</v>
+        <v>0.999960188316047</v>
       </c>
       <c r="G61" t="n">
-        <v>0.1907317912026389</v>
+        <v>3.107423372017367e-05</v>
       </c>
     </row>
     <row r="62">
@@ -2177,20 +2177,20 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.001127388612258672</v>
+        <v>3.4908234751866e-06</v>
       </c>
       <c r="E62" t="n">
-        <v>0.000607280839122441</v>
+        <v>0.000233904899877788</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0001837691372403923</v>
+        <v>0.946680597645899</v>
       </c>
       <c r="G62" t="n">
-        <v>0.9980815614113785</v>
+        <v>0.05308200663074798</v>
       </c>
     </row>
     <row r="63">
@@ -2206,20 +2206,20 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>incorrect sad</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>6.834589869962718e-05</v>
+        <v>1.023693455987201e-08</v>
       </c>
       <c r="E63" t="n">
-        <v>3.184100505104587e-07</v>
+        <v>0.0005019689715968527</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0001736866503709704</v>
+        <v>0.9424076118092418</v>
       </c>
       <c r="G63" t="n">
-        <v>0.9997576490408789</v>
+        <v>0.05709040898222684</v>
       </c>
     </row>
     <row r="64">
@@ -2235,20 +2235,20 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.9999999528990353</v>
+        <v>9.646660953670156e-07</v>
       </c>
       <c r="E64" t="n">
-        <v>5.381575366651896e-11</v>
+        <v>0.01706793888992523</v>
       </c>
       <c r="F64" t="n">
-        <v>4.699688018936161e-08</v>
+        <v>0.9825444045402338</v>
       </c>
       <c r="G64" t="n">
-        <v>5.026878163688254e-11</v>
+        <v>0.0003866919037454323</v>
       </c>
     </row>
     <row r="65">
@@ -2264,20 +2264,20 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.7079236613158439</v>
+        <v>2.472995244414275e-07</v>
       </c>
       <c r="E65" t="n">
-        <v>0.2108682833567001</v>
+        <v>0.0004702843442613148</v>
       </c>
       <c r="F65" t="n">
-        <v>0.01648694013784735</v>
+        <v>0.6533217909105644</v>
       </c>
       <c r="G65" t="n">
-        <v>0.06472111518960871</v>
+        <v>0.3462076774456499</v>
       </c>
     </row>
     <row r="66">
@@ -2293,20 +2293,20 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>1.271432008802708e-09</v>
+        <v>5.554746310560032e-06</v>
       </c>
       <c r="E66" t="n">
-        <v>0.006220609017639323</v>
+        <v>6.447403061902493e-05</v>
       </c>
       <c r="F66" t="n">
-        <v>0.9902612147676796</v>
+        <v>0.2238879632873996</v>
       </c>
       <c r="G66" t="n">
-        <v>0.003518174943248964</v>
+        <v>0.7760420079356708</v>
       </c>
     </row>
     <row r="67">
@@ -2322,20 +2322,20 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>incorrect neutral</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>7.661428444391292e-05</v>
+        <v>0.07006424990362049</v>
       </c>
       <c r="E67" t="n">
-        <v>0.006508288854685193</v>
+        <v>1.237441960632043e-05</v>
       </c>
       <c r="F67" t="n">
-        <v>0.9923101244304144</v>
+        <v>0.007920398153679542</v>
       </c>
       <c r="G67" t="n">
-        <v>0.001104972430456578</v>
+        <v>0.9220029775230937</v>
       </c>
     </row>
     <row r="68">
@@ -2351,20 +2351,20 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>incorrect happy</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.0001853634355038322</v>
+        <v>1.877051282124541e-07</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5952940679458123</v>
+        <v>3.271081722528107e-06</v>
       </c>
       <c r="F68" t="n">
-        <v>0.07617995639856043</v>
+        <v>0.0002584318526417894</v>
       </c>
       <c r="G68" t="n">
-        <v>0.3283406122201234</v>
+        <v>0.9997381093605073</v>
       </c>
     </row>
     <row r="69">
@@ -2384,16 +2384,16 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.04480768761962401</v>
+        <v>5.778812495844813e-09</v>
       </c>
       <c r="E69" t="n">
-        <v>0.01209984020494869</v>
+        <v>5.281718848022503e-06</v>
       </c>
       <c r="F69" t="n">
-        <v>0.0004834908433638238</v>
+        <v>0.0003642333232996924</v>
       </c>
       <c r="G69" t="n">
-        <v>0.9426089813320636</v>
+        <v>0.9996304791790398</v>
       </c>
     </row>
     <row r="70">
@@ -2413,16 +2413,16 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.2023756366291246</v>
+        <v>5.189162916037242e-11</v>
       </c>
       <c r="E70" t="n">
-        <v>0.05577092103123903</v>
+        <v>8.530014183711165e-08</v>
       </c>
       <c r="F70" t="n">
-        <v>0.0004469869472207065</v>
+        <v>6.466400372523764e-05</v>
       </c>
       <c r="G70" t="n">
-        <v>0.7414064553924157</v>
+        <v>0.9999352506442414</v>
       </c>
     </row>
     <row r="71">
@@ -2438,20 +2438,20 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>incorrect angry</t>
+          <t>correct</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.9448782099607397</v>
+        <v>1.092248634714955e-13</v>
       </c>
       <c r="E71" t="n">
-        <v>3.319323954054785e-05</v>
+        <v>1.114084551327302e-11</v>
       </c>
       <c r="F71" t="n">
-        <v>0.03612211234203849</v>
+        <v>0.0001767039769770367</v>
       </c>
       <c r="G71" t="n">
-        <v>0.01896648445768137</v>
+        <v>0.9998232960117728</v>
       </c>
     </row>
   </sheetData>

</xml_diff>